<commit_message>
Changed Invoice excel format to print pdf correctly #CRM-942
</commit_message>
<xml_diff>
--- a/application/controllers/excel-templates/247around_Tax_Invoice_Inter_State.xlsx
+++ b/application/controllers/excel-templates/247around_Tax_Invoice_Inter_State.xlsx
@@ -31,19 +31,19 @@
     <t>{meta:invoice_type}</t>
   </si>
   <si>
-    <t>Invoice No: {meta:invoice_id}</t>
+    <t xml:space="preserve"> Invoice No: {meta:invoice_id}</t>
   </si>
   <si>
     <t>Reference No: {meta:reference_invoice_id}</t>
   </si>
   <si>
-    <t>Date: {meta:invoice_date}</t>
+    <t xml:space="preserve"> Date: {meta:invoice_date} </t>
   </si>
   <si>
     <t>Period: {meta:sd} - {meta:ed}</t>
   </si>
   <si>
-    <t>Reverse Charge (Y/N):</t>
+    <t xml:space="preserve"> Reverse Charge (Y/N):</t>
   </si>
   <si>
     <t>N</t>
@@ -52,13 +52,13 @@
     <t>Bill to Party</t>
   </si>
   <si>
-    <t>Name: {meta:company_name}</t>
-  </si>
-  <si>
-    <t>Address: {meta:company_address}</t>
-  </si>
-  <si>
-    <t>GSTIN: {meta:gst_number}</t>
+    <t xml:space="preserve"> Name: {meta:company_name}</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Address: {meta:company_address}</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> GSTIN: {meta:gst_number}</t>
   </si>
   <si>
     <t>Place of Supply: {meta:state}</t>
@@ -92,7 +92,7 @@
     <t>Amount</t>
   </si>
   <si>
-    <t>{booking:description}</t>
+    <t xml:space="preserve"> {booking:description}</t>
   </si>
   <si>
     <t>{booking:hsn_code}</t>
@@ -180,7 +180,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="16">
+  <fonts count="15">
     <font>
       <sz val="11.0"/>
       <color rgb="FF000000"/>
@@ -188,7 +188,7 @@
     </font>
     <font>
       <b/>
-      <sz val="14.0"/>
+      <sz val="12.0"/>
       <color rgb="FF000000"/>
       <name val="Bookman Old Style"/>
     </font>
@@ -198,12 +198,6 @@
       <sz val="11.0"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12.0"/>
-      <color rgb="FF000000"/>
-      <name val="Bookman Old Style"/>
     </font>
     <font>
       <sz val="10.0"/>
@@ -245,18 +239,18 @@
     </font>
     <font>
       <b/>
+      <sz val="9.0"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
       <name val="Bookman Old Style"/>
     </font>
     <font>
       <sz val="10.0"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9.0"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
@@ -736,7 +730,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="98">
+  <cellXfs count="99">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -751,43 +745,43 @@
     <xf borderId="4" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
     <xf borderId="5" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="4" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf borderId="6" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="7" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="7" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="7" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf borderId="7" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="7" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf borderId="7" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="7" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="7" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf borderId="7" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -796,94 +790,97 @@
     <xf borderId="8" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="1" fillId="2" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf borderId="6" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="8" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="9" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf borderId="9" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="10" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="11" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="12" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="12" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf borderId="13" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="14" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="15" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf borderId="15" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="16" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="17" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="10" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="10" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf borderId="18" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="18" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="10" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="10" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" vertical="center"/>
     </xf>
-    <xf borderId="12" fillId="2" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="12" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="19" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
+    <xf borderId="19" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="20" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="21" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="22" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="23" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="24" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="19" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="19" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="20" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf borderId="20" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="25" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="26" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf borderId="25" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="26" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf borderId="1" fillId="2" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="27" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="28" fillId="2" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="28" fillId="2" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="29" fillId="2" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="28" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="30" fillId="2" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="29" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="30" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf borderId="31" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="29" fillId="2" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="29" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf borderId="32" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="33" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="34" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="35" fillId="2" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="35" fillId="2" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="36" fillId="2" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="36" fillId="2" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf borderId="37" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="4" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
+    <xf borderId="4" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="38" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="39" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="39" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="38" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="38" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf borderId="12" fillId="2" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -899,35 +896,35 @@
     <xf borderId="13" fillId="0" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="6" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="6" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="22" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="22" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf borderId="42" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="22" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="22" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="15" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="15" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf borderId="43" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="15" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="15" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="44" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="44" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf borderId="45" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="44" fillId="0" fontId="6" numFmtId="1" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="44" fillId="0" fontId="5" numFmtId="1" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf borderId="46" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="47" fillId="2" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="47" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf borderId="48" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
@@ -935,16 +932,16 @@
     <xf borderId="1" fillId="0" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="13" fillId="0" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="13" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf borderId="12" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="12" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf borderId="9" fillId="0" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="44" fillId="0" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -953,10 +950,10 @@
     <xf borderId="50" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="51" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="52" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -979,7 +976,7 @@
     <xdr:ext cx="400050" cy="466725"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image2.png"/>
+        <xdr:cNvPr id="0" name="image1.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -1007,7 +1004,7 @@
     <xdr:ext cx="1028700" cy="1143000"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image1.jpg" title="Image"/>
+        <xdr:cNvPr id="0" name="image2.jpg" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -1081,7 +1078,7 @@
     <col customWidth="1" min="14" max="14" width="4.29"/>
     <col customWidth="1" min="15" max="15" width="2.71"/>
     <col customWidth="1" min="16" max="16" width="3.86"/>
-    <col customWidth="1" min="17" max="17" width="3.14"/>
+    <col customWidth="1" min="17" max="17" width="5.14"/>
     <col customWidth="1" min="18" max="18" width="0.86"/>
   </cols>
   <sheetData>
@@ -1415,22 +1412,22 @@
       <c r="H16" s="51" t="s">
         <v>19</v>
       </c>
-      <c r="I16" s="51" t="s">
+      <c r="I16" s="52" t="s">
         <v>20</v>
       </c>
-      <c r="J16" s="51" t="s">
+      <c r="J16" s="52" t="s">
         <v>21</v>
       </c>
-      <c r="K16" s="52" t="s">
+      <c r="K16" s="53" t="s">
         <v>22</v>
       </c>
       <c r="L16" s="50"/>
-      <c r="M16" s="53" t="s">
+      <c r="M16" s="54" t="s">
         <v>23</v>
       </c>
       <c r="N16" s="27"/>
-      <c r="O16" s="54"/>
-      <c r="P16" s="55" t="s">
+      <c r="O16" s="55"/>
+      <c r="P16" s="56" t="s">
         <v>24</v>
       </c>
       <c r="Q16" s="4"/>
@@ -1443,50 +1440,50 @@
       <c r="D17" s="19"/>
       <c r="E17" s="19"/>
       <c r="F17" s="19"/>
-      <c r="G17" s="56"/>
-      <c r="H17" s="57"/>
-      <c r="I17" s="57"/>
-      <c r="J17" s="57"/>
-      <c r="K17" s="58"/>
-      <c r="L17" s="56"/>
-      <c r="M17" s="59" t="s">
+      <c r="G17" s="57"/>
+      <c r="H17" s="58"/>
+      <c r="I17" s="58"/>
+      <c r="J17" s="58"/>
+      <c r="K17" s="59"/>
+      <c r="L17" s="57"/>
+      <c r="M17" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="N17" s="60" t="s">
+      <c r="N17" s="61" t="s">
         <v>25</v>
       </c>
-      <c r="O17" s="61"/>
-      <c r="P17" s="58"/>
+      <c r="O17" s="62"/>
+      <c r="P17" s="59"/>
       <c r="Q17" s="25"/>
       <c r="R17" s="1"/>
     </row>
-    <row r="18" ht="28.5" customHeight="1">
+    <row r="18" ht="43.5" customHeight="1">
       <c r="A18" s="1"/>
-      <c r="B18" s="62" t="s">
+      <c r="B18" s="63" t="s">
         <v>26</v>
       </c>
-      <c r="G18" s="63"/>
-      <c r="H18" s="64" t="s">
+      <c r="G18" s="64"/>
+      <c r="H18" s="65" t="s">
         <v>27</v>
       </c>
-      <c r="I18" s="65" t="s">
+      <c r="I18" s="66" t="s">
         <v>28</v>
       </c>
-      <c r="J18" s="64" t="s">
+      <c r="J18" s="65" t="s">
         <v>29</v>
       </c>
-      <c r="K18" s="66" t="s">
+      <c r="K18" s="67" t="s">
         <v>30</v>
       </c>
-      <c r="L18" s="63"/>
-      <c r="M18" s="64" t="s">
+      <c r="L18" s="64"/>
+      <c r="M18" s="65" t="s">
         <v>31</v>
       </c>
-      <c r="N18" s="66" t="s">
+      <c r="N18" s="67" t="s">
         <v>32</v>
       </c>
-      <c r="O18" s="63"/>
-      <c r="P18" s="66" t="s">
+      <c r="O18" s="64"/>
+      <c r="P18" s="67" t="s">
         <v>33</v>
       </c>
       <c r="Q18" s="9"/>
@@ -1494,29 +1491,29 @@
     </row>
     <row r="19" ht="18.75" customHeight="1">
       <c r="A19" s="1"/>
-      <c r="B19" s="67" t="s">
+      <c r="B19" s="68" t="s">
         <v>24</v>
       </c>
       <c r="C19" s="30"/>
       <c r="D19" s="30"/>
       <c r="E19" s="30"/>
       <c r="F19" s="30"/>
-      <c r="G19" s="68"/>
-      <c r="H19" s="69"/>
-      <c r="I19" s="70" t="s">
+      <c r="G19" s="69"/>
+      <c r="H19" s="70"/>
+      <c r="I19" s="71" t="s">
         <v>34</v>
       </c>
-      <c r="J19" s="70"/>
-      <c r="K19" s="71" t="s">
+      <c r="J19" s="71"/>
+      <c r="K19" s="72" t="s">
         <v>35</v>
       </c>
-      <c r="L19" s="68"/>
-      <c r="M19" s="70"/>
-      <c r="N19" s="71" t="s">
+      <c r="L19" s="69"/>
+      <c r="M19" s="71"/>
+      <c r="N19" s="72" t="s">
         <v>36</v>
       </c>
-      <c r="O19" s="68"/>
-      <c r="P19" s="71" t="s">
+      <c r="O19" s="69"/>
+      <c r="P19" s="72" t="s">
         <v>37</v>
       </c>
       <c r="Q19" s="31"/>
@@ -1524,7 +1521,7 @@
     </row>
     <row r="20">
       <c r="A20" s="1"/>
-      <c r="B20" s="72" t="s">
+      <c r="B20" s="73" t="s">
         <v>38</v>
       </c>
       <c r="C20" s="19"/>
@@ -1535,14 +1532,14 @@
       <c r="H20" s="19"/>
       <c r="I20" s="19"/>
       <c r="J20" s="19"/>
-      <c r="K20" s="73" t="s">
+      <c r="K20" s="74" t="s">
         <v>39</v>
       </c>
       <c r="L20" s="43"/>
       <c r="M20" s="43"/>
       <c r="N20" s="43"/>
-      <c r="O20" s="74"/>
-      <c r="P20" s="75" t="s">
+      <c r="O20" s="75"/>
+      <c r="P20" s="76" t="s">
         <v>40</v>
       </c>
       <c r="Q20" s="44"/>
@@ -1550,7 +1547,7 @@
     </row>
     <row r="21" ht="15.75" customHeight="1">
       <c r="A21" s="1"/>
-      <c r="B21" s="76" t="s">
+      <c r="B21" s="77" t="s">
         <v>41</v>
       </c>
       <c r="C21" s="3"/>
@@ -1561,14 +1558,14 @@
       <c r="H21" s="3"/>
       <c r="I21" s="3"/>
       <c r="J21" s="4"/>
-      <c r="K21" s="77" t="s">
+      <c r="K21" s="78" t="s">
         <v>42</v>
       </c>
       <c r="L21" s="33"/>
       <c r="M21" s="33"/>
       <c r="N21" s="33"/>
-      <c r="O21" s="78"/>
-      <c r="P21" s="79" t="s">
+      <c r="O21" s="79"/>
+      <c r="P21" s="80" t="s">
         <v>43</v>
       </c>
       <c r="Q21" s="34"/>
@@ -1585,40 +1582,40 @@
       <c r="H22" s="19"/>
       <c r="I22" s="19"/>
       <c r="J22" s="25"/>
-      <c r="K22" s="80" t="s">
+      <c r="K22" s="81" t="s">
         <v>44</v>
       </c>
-      <c r="L22" s="81"/>
-      <c r="M22" s="81"/>
-      <c r="N22" s="81"/>
-      <c r="O22" s="61"/>
-      <c r="P22" s="82" t="s">
+      <c r="L22" s="82"/>
+      <c r="M22" s="82"/>
+      <c r="N22" s="82"/>
+      <c r="O22" s="62"/>
+      <c r="P22" s="83" t="s">
         <v>45</v>
       </c>
-      <c r="Q22" s="83"/>
+      <c r="Q22" s="84"/>
       <c r="R22" s="1"/>
     </row>
     <row r="23" ht="15.75" customHeight="1">
       <c r="A23" s="1"/>
-      <c r="B23" s="84" t="s">
+      <c r="B23" s="85" t="s">
         <v>46</v>
       </c>
-      <c r="C23" s="85"/>
-      <c r="D23" s="85"/>
-      <c r="E23" s="85"/>
-      <c r="F23" s="85"/>
-      <c r="G23" s="86"/>
-      <c r="H23" s="87"/>
+      <c r="C23" s="86"/>
+      <c r="D23" s="86"/>
+      <c r="E23" s="86"/>
+      <c r="F23" s="86"/>
+      <c r="G23" s="87"/>
+      <c r="H23" s="88"/>
       <c r="I23" s="3"/>
       <c r="J23" s="4"/>
-      <c r="K23" s="88" t="s">
+      <c r="K23" s="89" t="s">
         <v>47</v>
       </c>
       <c r="L23" s="30"/>
       <c r="M23" s="30"/>
       <c r="N23" s="30"/>
       <c r="O23" s="31"/>
-      <c r="P23" s="89">
+      <c r="P23" s="90">
         <f>IF(I10="Y",P21,0)</f>
         <v>0</v>
       </c>
@@ -1627,17 +1624,17 @@
     </row>
     <row r="24" ht="15.75" customHeight="1">
       <c r="A24" s="1"/>
-      <c r="B24" s="90" t="s">
+      <c r="B24" s="91" t="s">
         <v>48</v>
       </c>
       <c r="C24" s="27"/>
       <c r="D24" s="27"/>
       <c r="E24" s="27"/>
       <c r="F24" s="27"/>
-      <c r="G24" s="54"/>
+      <c r="G24" s="55"/>
       <c r="H24" s="10"/>
       <c r="J24" s="9"/>
-      <c r="K24" s="91" t="s">
+      <c r="K24" s="92" t="s">
         <v>49</v>
       </c>
       <c r="L24" s="3"/>
@@ -1650,38 +1647,38 @@
     </row>
     <row r="25" ht="15.75" customHeight="1">
       <c r="A25" s="1"/>
-      <c r="B25" s="92" t="s">
+      <c r="B25" s="93" t="s">
         <v>50</v>
       </c>
-      <c r="C25" s="81"/>
-      <c r="D25" s="81"/>
-      <c r="E25" s="81"/>
-      <c r="F25" s="81"/>
-      <c r="G25" s="61"/>
+      <c r="C25" s="82"/>
+      <c r="D25" s="82"/>
+      <c r="E25" s="82"/>
+      <c r="F25" s="82"/>
+      <c r="G25" s="62"/>
       <c r="H25" s="10"/>
       <c r="J25" s="9"/>
-      <c r="K25" s="93"/>
-      <c r="L25" s="94"/>
-      <c r="M25" s="94"/>
-      <c r="N25" s="94"/>
-      <c r="O25" s="94"/>
-      <c r="P25" s="94"/>
-      <c r="Q25" s="95"/>
+      <c r="K25" s="94"/>
+      <c r="L25" s="95"/>
+      <c r="M25" s="95"/>
+      <c r="N25" s="95"/>
+      <c r="O25" s="95"/>
+      <c r="P25" s="95"/>
+      <c r="Q25" s="96"/>
       <c r="R25" s="1"/>
     </row>
     <row r="26" ht="15.75" customHeight="1">
       <c r="A26" s="1"/>
-      <c r="B26" s="92" t="s">
+      <c r="B26" s="93" t="s">
         <v>51</v>
       </c>
-      <c r="C26" s="81"/>
-      <c r="D26" s="81"/>
-      <c r="E26" s="81"/>
-      <c r="F26" s="81"/>
-      <c r="G26" s="61"/>
+      <c r="C26" s="82"/>
+      <c r="D26" s="82"/>
+      <c r="E26" s="82"/>
+      <c r="F26" s="82"/>
+      <c r="G26" s="62"/>
       <c r="H26" s="10"/>
       <c r="J26" s="9"/>
-      <c r="K26" s="87"/>
+      <c r="K26" s="88"/>
       <c r="L26" s="3"/>
       <c r="M26" s="3"/>
       <c r="N26" s="3"/>
@@ -1692,7 +1689,7 @@
     </row>
     <row r="27" ht="15.75" customHeight="1">
       <c r="A27" s="1"/>
-      <c r="B27" s="96"/>
+      <c r="B27" s="97"/>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
       <c r="E27" s="3"/>
@@ -1740,7 +1737,7 @@
       <c r="H30" s="24"/>
       <c r="I30" s="19"/>
       <c r="J30" s="25"/>
-      <c r="K30" s="72" t="s">
+      <c r="K30" s="73" t="s">
         <v>52</v>
       </c>
       <c r="L30" s="19"/>
@@ -1772,7 +1769,7 @@
       <c r="R31" s="1"/>
     </row>
     <row r="32">
-      <c r="B32" s="97" t="s">
+      <c r="B32" s="98" t="s">
         <v>53</v>
       </c>
     </row>
@@ -2746,65 +2743,65 @@
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="55">
+    <mergeCell ref="I15:O15"/>
+    <mergeCell ref="B13:Q14"/>
+    <mergeCell ref="H16:H17"/>
+    <mergeCell ref="I16:I17"/>
+    <mergeCell ref="B10:H10"/>
+    <mergeCell ref="B11:Q11"/>
     <mergeCell ref="B16:G17"/>
     <mergeCell ref="B15:H15"/>
     <mergeCell ref="B9:I9"/>
-    <mergeCell ref="B8:I8"/>
     <mergeCell ref="K16:L17"/>
-    <mergeCell ref="I15:O15"/>
     <mergeCell ref="P15:Q15"/>
+    <mergeCell ref="P16:Q17"/>
+    <mergeCell ref="J16:J17"/>
+    <mergeCell ref="B12:Q12"/>
+    <mergeCell ref="K21:O21"/>
+    <mergeCell ref="K20:O20"/>
     <mergeCell ref="M16:O16"/>
     <mergeCell ref="N17:O17"/>
-    <mergeCell ref="P16:Q17"/>
-    <mergeCell ref="B13:Q14"/>
+    <mergeCell ref="K23:O23"/>
+    <mergeCell ref="P23:Q23"/>
+    <mergeCell ref="K24:Q25"/>
+    <mergeCell ref="K19:L19"/>
+    <mergeCell ref="K18:L18"/>
     <mergeCell ref="G4:M4"/>
     <mergeCell ref="F3:N3"/>
-    <mergeCell ref="B10:H10"/>
-    <mergeCell ref="J8:Q8"/>
     <mergeCell ref="B2:Q2"/>
     <mergeCell ref="G5:M5"/>
     <mergeCell ref="B3:C4"/>
     <mergeCell ref="O3:Q4"/>
+    <mergeCell ref="B8:I8"/>
+    <mergeCell ref="J8:Q8"/>
     <mergeCell ref="B6:Q7"/>
+    <mergeCell ref="K22:O22"/>
+    <mergeCell ref="P22:Q22"/>
+    <mergeCell ref="B21:J22"/>
+    <mergeCell ref="P21:Q21"/>
+    <mergeCell ref="B20:J20"/>
+    <mergeCell ref="P20:Q20"/>
+    <mergeCell ref="J9:Q9"/>
+    <mergeCell ref="J10:Q10"/>
+    <mergeCell ref="P18:Q18"/>
+    <mergeCell ref="N18:O18"/>
+    <mergeCell ref="B18:G18"/>
+    <mergeCell ref="P19:Q19"/>
+    <mergeCell ref="N19:O19"/>
+    <mergeCell ref="B19:G19"/>
+    <mergeCell ref="B23:G23"/>
+    <mergeCell ref="B24:G24"/>
     <mergeCell ref="K26:Q29"/>
-    <mergeCell ref="K23:O23"/>
-    <mergeCell ref="P23:Q23"/>
-    <mergeCell ref="K24:Q25"/>
-    <mergeCell ref="P19:Q19"/>
-    <mergeCell ref="P18:Q18"/>
     <mergeCell ref="K30:Q30"/>
     <mergeCell ref="B32:Q32"/>
     <mergeCell ref="B27:G30"/>
     <mergeCell ref="B26:G26"/>
     <mergeCell ref="H23:J30"/>
     <mergeCell ref="B25:G25"/>
-    <mergeCell ref="K22:O22"/>
-    <mergeCell ref="P22:Q22"/>
-    <mergeCell ref="K21:O21"/>
-    <mergeCell ref="B21:J22"/>
-    <mergeCell ref="P21:Q21"/>
-    <mergeCell ref="K20:O20"/>
-    <mergeCell ref="B20:J20"/>
-    <mergeCell ref="P20:Q20"/>
-    <mergeCell ref="J9:Q9"/>
-    <mergeCell ref="J10:Q10"/>
-    <mergeCell ref="K19:L19"/>
-    <mergeCell ref="H16:H17"/>
-    <mergeCell ref="I16:I17"/>
-    <mergeCell ref="J16:J17"/>
-    <mergeCell ref="N18:O18"/>
-    <mergeCell ref="K18:L18"/>
-    <mergeCell ref="N19:O19"/>
-    <mergeCell ref="B11:Q11"/>
-    <mergeCell ref="B12:Q12"/>
-    <mergeCell ref="B18:G18"/>
-    <mergeCell ref="B19:G19"/>
-    <mergeCell ref="B23:G23"/>
-    <mergeCell ref="B24:G24"/>
   </mergeCells>
-  <printOptions/>
+  <printOptions horizontalCentered="1"/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup orientation="landscape"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Defective parts return to partner #CRM-1120
</commit_message>
<xml_diff>
--- a/application/controllers/excel-templates/247around_Tax_Invoice_Inter_State.xlsx
+++ b/application/controllers/excel-templates/247around_Tax_Invoice_Inter_State.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/MAMP/htdocs/247around-adminp-aws/application/controllers/excel-templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{9E1BED21-5492-1145-B3B5-4CA61DF9B976}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{6C382440-7985-C84F-B238-AE638D356968}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Tax Invoice - Inter State" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Tax Invoice - Inter State'!$A$1:$R$32</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Tax Invoice - Inter State'!$A$1:$R$33</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
 </workbook>
@@ -936,41 +936,132 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="9" fillId="0" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -978,26 +1069,23 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1008,95 +1096,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="9" fillId="0" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1155,11 +1155,11 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>66675</xdr:colOff>
+      <xdr:colOff>282575</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:rowOff>12700</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="1028700" cy="1143000"/>
+    <xdr:ext cx="1139825" cy="1098550"/>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="3" name="image1.jpg" title="Image">
@@ -1178,6 +1178,10 @@
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2581275" y="5765800"/>
+          <a:ext cx="1139825" cy="1098550"/>
+        </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
@@ -1188,8 +1192,8 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>47625</xdr:colOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>149225</xdr:colOff>
       <xdr:row>25</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
@@ -1212,6 +1216,10 @@
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5000625" y="6334125"/>
+          <a:ext cx="1190625" cy="342900"/>
+        </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
@@ -1220,6 +1228,128 @@
     </xdr:pic>
     <xdr:clientData fLocksWithSheet="0"/>
   </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>88900</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>431800</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="1025" name="image2.png">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3F420887-C039-C941-9D44-1D07BF44FE3B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="152400" y="419100"/>
+          <a:ext cx="546100" cy="635000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>88900</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>431800</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="1026" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7153BCA5-B34E-3E4A-946C-27B68A7196B2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="152400" y="419100"/>
+          <a:ext cx="546100" cy="635000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1519,11 +1649,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:R1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5:M5"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13:Q14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1534,8 +1667,8 @@
     <col min="4" max="4" width="4.1640625" customWidth="1"/>
     <col min="5" max="5" width="5.33203125" customWidth="1"/>
     <col min="6" max="6" width="3.6640625" customWidth="1"/>
-    <col min="7" max="7" width="10.6640625" customWidth="1"/>
-    <col min="8" max="8" width="10.5" customWidth="1"/>
+    <col min="7" max="7" width="6.1640625" customWidth="1"/>
+    <col min="8" max="8" width="9.6640625" customWidth="1"/>
     <col min="9" max="9" width="6.1640625" customWidth="1"/>
     <col min="10" max="10" width="6.6640625" customWidth="1"/>
     <col min="11" max="11" width="1.1640625" customWidth="1"/>
@@ -1544,7 +1677,7 @@
     <col min="14" max="14" width="4.33203125" customWidth="1"/>
     <col min="15" max="15" width="6.1640625" customWidth="1"/>
     <col min="16" max="16" width="5.5" customWidth="1"/>
-    <col min="17" max="17" width="12" customWidth="1"/>
+    <col min="17" max="17" width="8.6640625" customWidth="1"/>
     <col min="18" max="18" width="0.83203125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1570,70 +1703,70 @@
     </row>
     <row r="2" spans="1:18" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
-      <c r="B2" s="48" t="s">
+      <c r="B2" s="73" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="26"/>
-      <c r="I2" s="26"/>
-      <c r="J2" s="26"/>
-      <c r="K2" s="26"/>
-      <c r="L2" s="26"/>
-      <c r="M2" s="26"/>
-      <c r="N2" s="26"/>
-      <c r="O2" s="26"/>
-      <c r="P2" s="26"/>
-      <c r="Q2" s="27"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="25"/>
+      <c r="J2" s="25"/>
+      <c r="K2" s="25"/>
+      <c r="L2" s="25"/>
+      <c r="M2" s="25"/>
+      <c r="N2" s="25"/>
+      <c r="O2" s="25"/>
+      <c r="P2" s="25"/>
+      <c r="Q2" s="37"/>
       <c r="R2" s="1"/>
     </row>
     <row r="3" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
-      <c r="B3" s="50"/>
-      <c r="C3" s="29"/>
+      <c r="B3" s="75"/>
+      <c r="C3" s="72"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
-      <c r="F3" s="47" t="s">
+      <c r="F3" s="71" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="29"/>
-      <c r="H3" s="29"/>
-      <c r="I3" s="29"/>
-      <c r="J3" s="29"/>
-      <c r="K3" s="29"/>
-      <c r="L3" s="29"/>
-      <c r="M3" s="29"/>
-      <c r="N3" s="29"/>
-      <c r="O3" s="51" t="s">
+      <c r="G3" s="72"/>
+      <c r="H3" s="72"/>
+      <c r="I3" s="72"/>
+      <c r="J3" s="72"/>
+      <c r="K3" s="72"/>
+      <c r="L3" s="72"/>
+      <c r="M3" s="72"/>
+      <c r="N3" s="72"/>
+      <c r="O3" s="77" t="s">
         <v>2</v>
       </c>
-      <c r="P3" s="29"/>
-      <c r="Q3" s="30"/>
+      <c r="P3" s="72"/>
+      <c r="Q3" s="78"/>
       <c r="R3" s="1"/>
     </row>
     <row r="4" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
-      <c r="B4" s="28"/>
-      <c r="C4" s="29"/>
+      <c r="B4" s="76"/>
+      <c r="C4" s="72"/>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
       <c r="F4" s="4"/>
-      <c r="G4" s="57" t="s">
+      <c r="G4" s="79" t="s">
         <v>3</v>
       </c>
-      <c r="H4" s="29"/>
-      <c r="I4" s="29"/>
-      <c r="J4" s="29"/>
-      <c r="K4" s="29"/>
-      <c r="L4" s="29"/>
-      <c r="M4" s="29"/>
+      <c r="H4" s="72"/>
+      <c r="I4" s="72"/>
+      <c r="J4" s="72"/>
+      <c r="K4" s="72"/>
+      <c r="L4" s="72"/>
+      <c r="M4" s="72"/>
       <c r="N4" s="5"/>
-      <c r="O4" s="29"/>
-      <c r="P4" s="29"/>
-      <c r="Q4" s="30"/>
+      <c r="O4" s="72"/>
+      <c r="P4" s="72"/>
+      <c r="Q4" s="78"/>
       <c r="R4" s="1"/>
     </row>
     <row r="5" spans="1:18" ht="16" x14ac:dyDescent="0.2">
@@ -1643,15 +1776,15 @@
       <c r="D5" s="8"/>
       <c r="E5" s="8"/>
       <c r="F5" s="8"/>
-      <c r="G5" s="49" t="s">
+      <c r="G5" s="74" t="s">
         <v>4</v>
       </c>
-      <c r="H5" s="32"/>
-      <c r="I5" s="32"/>
-      <c r="J5" s="32"/>
-      <c r="K5" s="32"/>
-      <c r="L5" s="32"/>
-      <c r="M5" s="32"/>
+      <c r="H5" s="28"/>
+      <c r="I5" s="28"/>
+      <c r="J5" s="28"/>
+      <c r="K5" s="28"/>
+      <c r="L5" s="28"/>
+      <c r="M5" s="28"/>
       <c r="N5" s="9"/>
       <c r="O5" s="9"/>
       <c r="P5" s="10"/>
@@ -1660,298 +1793,298 @@
     </row>
     <row r="6" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1"/>
-      <c r="B6" s="60" t="s">
+      <c r="B6" s="52" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="26"/>
-      <c r="D6" s="26"/>
-      <c r="E6" s="26"/>
-      <c r="F6" s="26"/>
-      <c r="G6" s="26"/>
-      <c r="H6" s="26"/>
-      <c r="I6" s="26"/>
-      <c r="J6" s="26"/>
-      <c r="K6" s="26"/>
-      <c r="L6" s="26"/>
-      <c r="M6" s="26"/>
-      <c r="N6" s="26"/>
-      <c r="O6" s="26"/>
-      <c r="P6" s="26"/>
-      <c r="Q6" s="27"/>
+      <c r="C6" s="25"/>
+      <c r="D6" s="25"/>
+      <c r="E6" s="25"/>
+      <c r="F6" s="25"/>
+      <c r="G6" s="25"/>
+      <c r="H6" s="25"/>
+      <c r="I6" s="25"/>
+      <c r="J6" s="25"/>
+      <c r="K6" s="25"/>
+      <c r="L6" s="25"/>
+      <c r="M6" s="25"/>
+      <c r="N6" s="25"/>
+      <c r="O6" s="25"/>
+      <c r="P6" s="25"/>
+      <c r="Q6" s="37"/>
       <c r="R6" s="1"/>
     </row>
     <row r="7" spans="1:18" ht="7.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1"/>
-      <c r="B7" s="31"/>
-      <c r="C7" s="32"/>
-      <c r="D7" s="32"/>
-      <c r="E7" s="32"/>
-      <c r="F7" s="32"/>
-      <c r="G7" s="32"/>
-      <c r="H7" s="32"/>
-      <c r="I7" s="32"/>
-      <c r="J7" s="32"/>
-      <c r="K7" s="32"/>
-      <c r="L7" s="32"/>
-      <c r="M7" s="32"/>
-      <c r="N7" s="32"/>
-      <c r="O7" s="32"/>
-      <c r="P7" s="32"/>
-      <c r="Q7" s="33"/>
+      <c r="B7" s="27"/>
+      <c r="C7" s="28"/>
+      <c r="D7" s="28"/>
+      <c r="E7" s="28"/>
+      <c r="F7" s="28"/>
+      <c r="G7" s="28"/>
+      <c r="H7" s="28"/>
+      <c r="I7" s="28"/>
+      <c r="J7" s="28"/>
+      <c r="K7" s="28"/>
+      <c r="L7" s="28"/>
+      <c r="M7" s="28"/>
+      <c r="N7" s="28"/>
+      <c r="O7" s="28"/>
+      <c r="P7" s="28"/>
+      <c r="Q7" s="38"/>
       <c r="R7" s="1"/>
     </row>
     <row r="8" spans="1:18" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1"/>
-      <c r="B8" s="22" t="s">
+      <c r="B8" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="23"/>
-      <c r="D8" s="23"/>
-      <c r="E8" s="23"/>
-      <c r="F8" s="23"/>
-      <c r="G8" s="23"/>
-      <c r="H8" s="23"/>
-      <c r="I8" s="58"/>
-      <c r="J8" s="59" t="s">
+      <c r="C8" s="42"/>
+      <c r="D8" s="42"/>
+      <c r="E8" s="42"/>
+      <c r="F8" s="42"/>
+      <c r="G8" s="42"/>
+      <c r="H8" s="42"/>
+      <c r="I8" s="43"/>
+      <c r="J8" s="51" t="s">
         <v>7</v>
       </c>
-      <c r="K8" s="46"/>
-      <c r="L8" s="46"/>
-      <c r="M8" s="46"/>
-      <c r="N8" s="46"/>
-      <c r="O8" s="46"/>
-      <c r="P8" s="46"/>
-      <c r="Q8" s="43"/>
+      <c r="K8" s="22"/>
+      <c r="L8" s="22"/>
+      <c r="M8" s="22"/>
+      <c r="N8" s="22"/>
+      <c r="O8" s="22"/>
+      <c r="P8" s="22"/>
+      <c r="Q8" s="23"/>
       <c r="R8" s="1"/>
     </row>
     <row r="9" spans="1:18" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1"/>
-      <c r="B9" s="79" t="s">
+      <c r="B9" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="71"/>
-      <c r="D9" s="71"/>
-      <c r="E9" s="71"/>
-      <c r="F9" s="71"/>
-      <c r="G9" s="71"/>
-      <c r="H9" s="71"/>
-      <c r="I9" s="66"/>
-      <c r="J9" s="69" t="s">
+      <c r="C9" s="20"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="20"/>
+      <c r="H9" s="20"/>
+      <c r="I9" s="60"/>
+      <c r="J9" s="63" t="s">
         <v>9</v>
       </c>
-      <c r="K9" s="23"/>
-      <c r="L9" s="23"/>
-      <c r="M9" s="23"/>
-      <c r="N9" s="23"/>
-      <c r="O9" s="23"/>
-      <c r="P9" s="23"/>
-      <c r="Q9" s="58"/>
+      <c r="K9" s="42"/>
+      <c r="L9" s="42"/>
+      <c r="M9" s="42"/>
+      <c r="N9" s="42"/>
+      <c r="O9" s="42"/>
+      <c r="P9" s="42"/>
+      <c r="Q9" s="43"/>
       <c r="R9" s="1"/>
     </row>
     <row r="10" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1"/>
-      <c r="B10" s="79" t="s">
+      <c r="B10" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="71"/>
-      <c r="D10" s="71"/>
-      <c r="E10" s="71"/>
-      <c r="F10" s="71"/>
-      <c r="G10" s="71"/>
-      <c r="H10" s="71"/>
+      <c r="C10" s="20"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="20"/>
+      <c r="H10" s="20"/>
       <c r="I10" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="J10" s="69"/>
-      <c r="K10" s="23"/>
-      <c r="L10" s="23"/>
-      <c r="M10" s="23"/>
-      <c r="N10" s="23"/>
-      <c r="O10" s="23"/>
-      <c r="P10" s="23"/>
-      <c r="Q10" s="58"/>
+      <c r="J10" s="63"/>
+      <c r="K10" s="42"/>
+      <c r="L10" s="42"/>
+      <c r="M10" s="42"/>
+      <c r="N10" s="42"/>
+      <c r="O10" s="42"/>
+      <c r="P10" s="42"/>
+      <c r="Q10" s="43"/>
       <c r="R10" s="1"/>
     </row>
     <row r="11" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A11" s="1"/>
-      <c r="B11" s="95" t="s">
+      <c r="B11" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="46"/>
-      <c r="D11" s="46"/>
-      <c r="E11" s="46"/>
-      <c r="F11" s="46"/>
-      <c r="G11" s="46"/>
-      <c r="H11" s="46"/>
-      <c r="I11" s="46"/>
-      <c r="J11" s="46"/>
-      <c r="K11" s="46"/>
-      <c r="L11" s="46"/>
-      <c r="M11" s="46"/>
-      <c r="N11" s="46"/>
-      <c r="O11" s="46"/>
-      <c r="P11" s="46"/>
-      <c r="Q11" s="43"/>
+      <c r="C11" s="22"/>
+      <c r="D11" s="22"/>
+      <c r="E11" s="22"/>
+      <c r="F11" s="22"/>
+      <c r="G11" s="22"/>
+      <c r="H11" s="22"/>
+      <c r="I11" s="22"/>
+      <c r="J11" s="22"/>
+      <c r="K11" s="22"/>
+      <c r="L11" s="22"/>
+      <c r="M11" s="22"/>
+      <c r="N11" s="22"/>
+      <c r="O11" s="22"/>
+      <c r="P11" s="22"/>
+      <c r="Q11" s="23"/>
       <c r="R11" s="1"/>
     </row>
     <row r="12" spans="1:18" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1"/>
-      <c r="B12" s="22" t="s">
+      <c r="B12" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="23"/>
-      <c r="D12" s="23"/>
-      <c r="E12" s="23"/>
-      <c r="F12" s="23"/>
-      <c r="G12" s="23"/>
-      <c r="H12" s="23"/>
-      <c r="I12" s="23"/>
-      <c r="J12" s="23"/>
-      <c r="K12" s="23"/>
-      <c r="L12" s="23"/>
-      <c r="M12" s="23"/>
-      <c r="N12" s="23"/>
-      <c r="O12" s="23"/>
-      <c r="P12" s="23"/>
-      <c r="Q12" s="58"/>
+      <c r="C12" s="42"/>
+      <c r="D12" s="42"/>
+      <c r="E12" s="42"/>
+      <c r="F12" s="42"/>
+      <c r="G12" s="42"/>
+      <c r="H12" s="42"/>
+      <c r="I12" s="42"/>
+      <c r="J12" s="42"/>
+      <c r="K12" s="42"/>
+      <c r="L12" s="42"/>
+      <c r="M12" s="42"/>
+      <c r="N12" s="42"/>
+      <c r="O12" s="42"/>
+      <c r="P12" s="42"/>
+      <c r="Q12" s="43"/>
       <c r="R12" s="1"/>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A13" s="1"/>
-      <c r="B13" s="92" t="s">
+      <c r="B13" s="46" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="90"/>
-      <c r="D13" s="90"/>
-      <c r="E13" s="90"/>
-      <c r="F13" s="90"/>
-      <c r="G13" s="90"/>
-      <c r="H13" s="90"/>
-      <c r="I13" s="90"/>
-      <c r="J13" s="90"/>
-      <c r="K13" s="90"/>
-      <c r="L13" s="90"/>
-      <c r="M13" s="90"/>
-      <c r="N13" s="90"/>
-      <c r="O13" s="90"/>
-      <c r="P13" s="90"/>
-      <c r="Q13" s="85"/>
+      <c r="C13" s="31"/>
+      <c r="D13" s="31"/>
+      <c r="E13" s="31"/>
+      <c r="F13" s="31"/>
+      <c r="G13" s="31"/>
+      <c r="H13" s="31"/>
+      <c r="I13" s="31"/>
+      <c r="J13" s="31"/>
+      <c r="K13" s="31"/>
+      <c r="L13" s="31"/>
+      <c r="M13" s="31"/>
+      <c r="N13" s="31"/>
+      <c r="O13" s="31"/>
+      <c r="P13" s="31"/>
+      <c r="Q13" s="35"/>
       <c r="R13" s="1"/>
     </row>
     <row r="14" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1"/>
-      <c r="B14" s="93"/>
-      <c r="C14" s="74"/>
-      <c r="D14" s="74"/>
-      <c r="E14" s="74"/>
-      <c r="F14" s="74"/>
-      <c r="G14" s="74"/>
-      <c r="H14" s="74"/>
-      <c r="I14" s="74"/>
-      <c r="J14" s="74"/>
-      <c r="K14" s="74"/>
-      <c r="L14" s="74"/>
-      <c r="M14" s="74"/>
-      <c r="N14" s="74"/>
-      <c r="O14" s="74"/>
-      <c r="P14" s="74"/>
-      <c r="Q14" s="68"/>
+      <c r="B14" s="47"/>
+      <c r="C14" s="48"/>
+      <c r="D14" s="48"/>
+      <c r="E14" s="48"/>
+      <c r="F14" s="48"/>
+      <c r="G14" s="48"/>
+      <c r="H14" s="48"/>
+      <c r="I14" s="48"/>
+      <c r="J14" s="48"/>
+      <c r="K14" s="48"/>
+      <c r="L14" s="48"/>
+      <c r="M14" s="48"/>
+      <c r="N14" s="48"/>
+      <c r="O14" s="48"/>
+      <c r="P14" s="48"/>
+      <c r="Q14" s="49"/>
       <c r="R14" s="1"/>
     </row>
     <row r="15" spans="1:18" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="1"/>
-      <c r="B15" s="97" t="s">
+      <c r="B15" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="90"/>
-      <c r="D15" s="90"/>
-      <c r="E15" s="90"/>
-      <c r="F15" s="90"/>
-      <c r="G15" s="90"/>
-      <c r="H15" s="90"/>
-      <c r="I15" s="89" t="s">
+      <c r="C15" s="31"/>
+      <c r="D15" s="31"/>
+      <c r="E15" s="31"/>
+      <c r="F15" s="31"/>
+      <c r="G15" s="31"/>
+      <c r="H15" s="31"/>
+      <c r="I15" s="44" t="s">
         <v>16</v>
       </c>
-      <c r="J15" s="90"/>
-      <c r="K15" s="90"/>
-      <c r="L15" s="90"/>
-      <c r="M15" s="90"/>
-      <c r="N15" s="90"/>
-      <c r="O15" s="91"/>
-      <c r="P15" s="84" t="s">
+      <c r="J15" s="31"/>
+      <c r="K15" s="31"/>
+      <c r="L15" s="31"/>
+      <c r="M15" s="31"/>
+      <c r="N15" s="31"/>
+      <c r="O15" s="45"/>
+      <c r="P15" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="Q15" s="85"/>
+      <c r="Q15" s="35"/>
       <c r="R15" s="1"/>
     </row>
     <row r="16" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="A16" s="1"/>
-      <c r="B16" s="96" t="s">
+      <c r="B16" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="C16" s="26"/>
-      <c r="D16" s="26"/>
-      <c r="E16" s="26"/>
-      <c r="F16" s="26"/>
-      <c r="G16" s="81"/>
-      <c r="H16" s="94" t="s">
+      <c r="C16" s="25"/>
+      <c r="D16" s="25"/>
+      <c r="E16" s="25"/>
+      <c r="F16" s="25"/>
+      <c r="G16" s="26"/>
+      <c r="H16" s="50" t="s">
         <v>19</v>
       </c>
-      <c r="I16" s="87" t="s">
+      <c r="I16" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="J16" s="87" t="s">
+      <c r="J16" s="39" t="s">
         <v>21</v>
       </c>
-      <c r="K16" s="80" t="s">
+      <c r="K16" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="L16" s="81"/>
-      <c r="M16" s="76" t="s">
+      <c r="L16" s="26"/>
+      <c r="M16" s="68" t="s">
         <v>23</v>
       </c>
-      <c r="N16" s="23"/>
-      <c r="O16" s="24"/>
-      <c r="P16" s="86" t="s">
+      <c r="N16" s="42"/>
+      <c r="O16" s="69"/>
+      <c r="P16" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="Q16" s="27"/>
+      <c r="Q16" s="37"/>
       <c r="R16" s="1"/>
     </row>
     <row r="17" spans="1:18" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="1"/>
-      <c r="B17" s="31"/>
-      <c r="C17" s="32"/>
-      <c r="D17" s="32"/>
-      <c r="E17" s="32"/>
-      <c r="F17" s="32"/>
-      <c r="G17" s="83"/>
-      <c r="H17" s="88"/>
-      <c r="I17" s="88"/>
-      <c r="J17" s="88"/>
-      <c r="K17" s="82"/>
-      <c r="L17" s="83"/>
+      <c r="B17" s="27"/>
+      <c r="C17" s="28"/>
+      <c r="D17" s="28"/>
+      <c r="E17" s="28"/>
+      <c r="F17" s="28"/>
+      <c r="G17" s="29"/>
+      <c r="H17" s="40"/>
+      <c r="I17" s="40"/>
+      <c r="J17" s="40"/>
+      <c r="K17" s="33"/>
+      <c r="L17" s="29"/>
       <c r="M17" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="N17" s="77" t="s">
+      <c r="N17" s="70" t="s">
         <v>25</v>
       </c>
-      <c r="O17" s="39"/>
-      <c r="P17" s="82"/>
-      <c r="Q17" s="33"/>
+      <c r="O17" s="55"/>
+      <c r="P17" s="33"/>
+      <c r="Q17" s="38"/>
       <c r="R17" s="1"/>
     </row>
     <row r="18" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="1"/>
-      <c r="B18" s="41" t="s">
+      <c r="B18" s="82" t="s">
         <v>26</v>
       </c>
-      <c r="C18" s="29"/>
-      <c r="D18" s="29"/>
-      <c r="E18" s="29"/>
-      <c r="F18" s="29"/>
-      <c r="G18" s="40"/>
+      <c r="C18" s="72"/>
+      <c r="D18" s="72"/>
+      <c r="E18" s="72"/>
+      <c r="F18" s="72"/>
+      <c r="G18" s="81"/>
       <c r="H18" s="14" t="s">
         <v>27</v>
       </c>
@@ -1961,304 +2094,304 @@
       <c r="J18" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="K18" s="35" t="s">
+      <c r="K18" s="80" t="s">
         <v>30</v>
       </c>
-      <c r="L18" s="40"/>
+      <c r="L18" s="81"/>
       <c r="M18" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="N18" s="35" t="s">
+      <c r="N18" s="80" t="s">
         <v>32</v>
       </c>
-      <c r="O18" s="40"/>
-      <c r="P18" s="35" t="s">
+      <c r="O18" s="81"/>
+      <c r="P18" s="80" t="s">
         <v>33</v>
       </c>
-      <c r="Q18" s="30"/>
+      <c r="Q18" s="78"/>
       <c r="R18" s="1"/>
     </row>
     <row r="19" spans="1:18" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="1"/>
-      <c r="B19" s="45" t="s">
+      <c r="B19" s="85" t="s">
         <v>24</v>
       </c>
-      <c r="C19" s="46"/>
-      <c r="D19" s="46"/>
-      <c r="E19" s="46"/>
-      <c r="F19" s="46"/>
-      <c r="G19" s="44"/>
+      <c r="C19" s="22"/>
+      <c r="D19" s="22"/>
+      <c r="E19" s="22"/>
+      <c r="F19" s="22"/>
+      <c r="G19" s="84"/>
       <c r="H19" s="16"/>
       <c r="I19" s="17" t="s">
         <v>34</v>
       </c>
       <c r="J19" s="17"/>
-      <c r="K19" s="42" t="s">
+      <c r="K19" s="83" t="s">
         <v>35</v>
       </c>
-      <c r="L19" s="44"/>
+      <c r="L19" s="84"/>
       <c r="M19" s="17"/>
-      <c r="N19" s="42" t="s">
+      <c r="N19" s="83" t="s">
         <v>36</v>
       </c>
-      <c r="O19" s="44"/>
-      <c r="P19" s="42" t="s">
+      <c r="O19" s="84"/>
+      <c r="P19" s="83" t="s">
         <v>37</v>
       </c>
-      <c r="Q19" s="43"/>
+      <c r="Q19" s="23"/>
       <c r="R19" s="1"/>
     </row>
     <row r="20" spans="1:18" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="1"/>
-      <c r="B20" s="34" t="s">
+      <c r="B20" s="61" t="s">
         <v>38</v>
       </c>
-      <c r="C20" s="32"/>
-      <c r="D20" s="32"/>
-      <c r="E20" s="32"/>
-      <c r="F20" s="32"/>
-      <c r="G20" s="32"/>
-      <c r="H20" s="32"/>
-      <c r="I20" s="32"/>
-      <c r="J20" s="32"/>
-      <c r="K20" s="73" t="s">
+      <c r="C20" s="28"/>
+      <c r="D20" s="28"/>
+      <c r="E20" s="28"/>
+      <c r="F20" s="28"/>
+      <c r="G20" s="28"/>
+      <c r="H20" s="28"/>
+      <c r="I20" s="28"/>
+      <c r="J20" s="28"/>
+      <c r="K20" s="66" t="s">
         <v>39</v>
       </c>
-      <c r="L20" s="74"/>
-      <c r="M20" s="74"/>
-      <c r="N20" s="74"/>
-      <c r="O20" s="75"/>
-      <c r="P20" s="67" t="s">
+      <c r="L20" s="48"/>
+      <c r="M20" s="48"/>
+      <c r="N20" s="48"/>
+      <c r="O20" s="67"/>
+      <c r="P20" s="62" t="s">
         <v>40</v>
       </c>
-      <c r="Q20" s="68"/>
+      <c r="Q20" s="49"/>
       <c r="R20" s="1"/>
     </row>
     <row r="21" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="1"/>
-      <c r="B21" s="64" t="s">
+      <c r="B21" s="58" t="s">
         <v>41</v>
       </c>
-      <c r="C21" s="26"/>
-      <c r="D21" s="26"/>
-      <c r="E21" s="26"/>
-      <c r="F21" s="26"/>
-      <c r="G21" s="26"/>
-      <c r="H21" s="26"/>
-      <c r="I21" s="26"/>
-      <c r="J21" s="27"/>
-      <c r="K21" s="70" t="s">
+      <c r="C21" s="25"/>
+      <c r="D21" s="25"/>
+      <c r="E21" s="25"/>
+      <c r="F21" s="25"/>
+      <c r="G21" s="25"/>
+      <c r="H21" s="25"/>
+      <c r="I21" s="25"/>
+      <c r="J21" s="37"/>
+      <c r="K21" s="64" t="s">
         <v>42</v>
       </c>
-      <c r="L21" s="71"/>
-      <c r="M21" s="71"/>
-      <c r="N21" s="71"/>
-      <c r="O21" s="72"/>
-      <c r="P21" s="65" t="s">
+      <c r="L21" s="20"/>
+      <c r="M21" s="20"/>
+      <c r="N21" s="20"/>
+      <c r="O21" s="65"/>
+      <c r="P21" s="59" t="s">
         <v>43</v>
       </c>
-      <c r="Q21" s="66"/>
+      <c r="Q21" s="60"/>
       <c r="R21" s="1"/>
     </row>
     <row r="22" spans="1:18" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="1"/>
-      <c r="B22" s="31"/>
-      <c r="C22" s="32"/>
-      <c r="D22" s="32"/>
-      <c r="E22" s="32"/>
-      <c r="F22" s="32"/>
-      <c r="G22" s="32"/>
-      <c r="H22" s="32"/>
-      <c r="I22" s="32"/>
-      <c r="J22" s="33"/>
-      <c r="K22" s="61" t="s">
+      <c r="B22" s="27"/>
+      <c r="C22" s="28"/>
+      <c r="D22" s="28"/>
+      <c r="E22" s="28"/>
+      <c r="F22" s="28"/>
+      <c r="G22" s="28"/>
+      <c r="H22" s="28"/>
+      <c r="I22" s="28"/>
+      <c r="J22" s="38"/>
+      <c r="K22" s="53" t="s">
         <v>44</v>
       </c>
-      <c r="L22" s="38"/>
-      <c r="M22" s="38"/>
-      <c r="N22" s="38"/>
-      <c r="O22" s="39"/>
-      <c r="P22" s="62" t="s">
+      <c r="L22" s="54"/>
+      <c r="M22" s="54"/>
+      <c r="N22" s="54"/>
+      <c r="O22" s="55"/>
+      <c r="P22" s="56" t="s">
         <v>45</v>
       </c>
-      <c r="Q22" s="63"/>
+      <c r="Q22" s="57"/>
       <c r="R22" s="1"/>
     </row>
     <row r="23" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="1"/>
-      <c r="B23" s="19" t="s">
+      <c r="B23" s="86" t="s">
         <v>46</v>
       </c>
-      <c r="C23" s="20"/>
-      <c r="D23" s="20"/>
-      <c r="E23" s="20"/>
-      <c r="F23" s="20"/>
-      <c r="G23" s="21"/>
-      <c r="H23" s="25"/>
-      <c r="I23" s="26"/>
-      <c r="J23" s="27"/>
-      <c r="K23" s="78" t="s">
+      <c r="C23" s="87"/>
+      <c r="D23" s="87"/>
+      <c r="E23" s="87"/>
+      <c r="F23" s="87"/>
+      <c r="G23" s="88"/>
+      <c r="H23" s="89"/>
+      <c r="I23" s="25"/>
+      <c r="J23" s="37"/>
+      <c r="K23" s="97" t="s">
         <v>47</v>
       </c>
-      <c r="L23" s="46"/>
-      <c r="M23" s="46"/>
-      <c r="N23" s="46"/>
-      <c r="O23" s="43"/>
-      <c r="P23" s="52">
+      <c r="L23" s="22"/>
+      <c r="M23" s="22"/>
+      <c r="N23" s="22"/>
+      <c r="O23" s="23"/>
+      <c r="P23" s="92">
         <f>IF(I10="Y",P21,0)</f>
         <v>0</v>
       </c>
-      <c r="Q23" s="43"/>
+      <c r="Q23" s="23"/>
       <c r="R23" s="1"/>
     </row>
     <row r="24" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="1"/>
-      <c r="B24" s="22" t="s">
+      <c r="B24" s="41" t="s">
         <v>48</v>
       </c>
-      <c r="C24" s="23"/>
-      <c r="D24" s="23"/>
-      <c r="E24" s="23"/>
-      <c r="F24" s="23"/>
-      <c r="G24" s="24"/>
-      <c r="H24" s="28"/>
-      <c r="I24" s="29"/>
-      <c r="J24" s="30"/>
-      <c r="K24" s="53" t="s">
+      <c r="C24" s="42"/>
+      <c r="D24" s="42"/>
+      <c r="E24" s="42"/>
+      <c r="F24" s="42"/>
+      <c r="G24" s="69"/>
+      <c r="H24" s="76"/>
+      <c r="I24" s="72"/>
+      <c r="J24" s="78"/>
+      <c r="K24" s="93" t="s">
         <v>49</v>
       </c>
-      <c r="L24" s="26"/>
-      <c r="M24" s="26"/>
-      <c r="N24" s="26"/>
-      <c r="O24" s="26"/>
-      <c r="P24" s="26"/>
-      <c r="Q24" s="27"/>
+      <c r="L24" s="25"/>
+      <c r="M24" s="25"/>
+      <c r="N24" s="25"/>
+      <c r="O24" s="25"/>
+      <c r="P24" s="25"/>
+      <c r="Q24" s="37"/>
       <c r="R24" s="1"/>
     </row>
     <row r="25" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="1"/>
-      <c r="B25" s="37" t="s">
+      <c r="B25" s="91" t="s">
         <v>50</v>
       </c>
-      <c r="C25" s="38"/>
-      <c r="D25" s="38"/>
-      <c r="E25" s="38"/>
-      <c r="F25" s="38"/>
-      <c r="G25" s="39"/>
-      <c r="H25" s="28"/>
-      <c r="I25" s="29"/>
-      <c r="J25" s="30"/>
-      <c r="K25" s="54"/>
-      <c r="L25" s="55"/>
-      <c r="M25" s="55"/>
-      <c r="N25" s="55"/>
-      <c r="O25" s="55"/>
-      <c r="P25" s="55"/>
-      <c r="Q25" s="56"/>
+      <c r="C25" s="54"/>
+      <c r="D25" s="54"/>
+      <c r="E25" s="54"/>
+      <c r="F25" s="54"/>
+      <c r="G25" s="55"/>
+      <c r="H25" s="76"/>
+      <c r="I25" s="72"/>
+      <c r="J25" s="78"/>
+      <c r="K25" s="94"/>
+      <c r="L25" s="95"/>
+      <c r="M25" s="95"/>
+      <c r="N25" s="95"/>
+      <c r="O25" s="95"/>
+      <c r="P25" s="95"/>
+      <c r="Q25" s="96"/>
       <c r="R25" s="1"/>
     </row>
     <row r="26" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="1"/>
-      <c r="B26" s="37" t="s">
+      <c r="B26" s="91" t="s">
         <v>51</v>
       </c>
-      <c r="C26" s="38"/>
-      <c r="D26" s="38"/>
-      <c r="E26" s="38"/>
-      <c r="F26" s="38"/>
-      <c r="G26" s="39"/>
-      <c r="H26" s="28"/>
-      <c r="I26" s="29"/>
-      <c r="J26" s="30"/>
-      <c r="K26" s="25"/>
-      <c r="L26" s="26"/>
-      <c r="M26" s="26"/>
-      <c r="N26" s="26"/>
-      <c r="O26" s="26"/>
-      <c r="P26" s="26"/>
-      <c r="Q26" s="27"/>
+      <c r="C26" s="54"/>
+      <c r="D26" s="54"/>
+      <c r="E26" s="54"/>
+      <c r="F26" s="54"/>
+      <c r="G26" s="55"/>
+      <c r="H26" s="76"/>
+      <c r="I26" s="72"/>
+      <c r="J26" s="78"/>
+      <c r="K26" s="89"/>
+      <c r="L26" s="25"/>
+      <c r="M26" s="25"/>
+      <c r="N26" s="25"/>
+      <c r="O26" s="25"/>
+      <c r="P26" s="25"/>
+      <c r="Q26" s="37"/>
       <c r="R26" s="1"/>
     </row>
     <row r="27" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="1"/>
-      <c r="B27" s="36"/>
-      <c r="C27" s="26"/>
-      <c r="D27" s="26"/>
-      <c r="E27" s="26"/>
-      <c r="F27" s="26"/>
-      <c r="G27" s="27"/>
-      <c r="H27" s="28"/>
-      <c r="I27" s="29"/>
-      <c r="J27" s="30"/>
-      <c r="K27" s="28"/>
-      <c r="L27" s="29"/>
-      <c r="M27" s="29"/>
-      <c r="N27" s="29"/>
-      <c r="O27" s="29"/>
-      <c r="P27" s="29"/>
-      <c r="Q27" s="30"/>
+      <c r="B27" s="90"/>
+      <c r="C27" s="25"/>
+      <c r="D27" s="25"/>
+      <c r="E27" s="25"/>
+      <c r="F27" s="25"/>
+      <c r="G27" s="37"/>
+      <c r="H27" s="76"/>
+      <c r="I27" s="72"/>
+      <c r="J27" s="78"/>
+      <c r="K27" s="76"/>
+      <c r="L27" s="72"/>
+      <c r="M27" s="72"/>
+      <c r="N27" s="72"/>
+      <c r="O27" s="72"/>
+      <c r="P27" s="72"/>
+      <c r="Q27" s="78"/>
       <c r="R27" s="1"/>
     </row>
     <row r="28" spans="1:18" ht="3.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="1"/>
-      <c r="B28" s="28"/>
-      <c r="C28" s="29"/>
-      <c r="D28" s="29"/>
-      <c r="E28" s="29"/>
-      <c r="F28" s="29"/>
-      <c r="G28" s="30"/>
-      <c r="H28" s="28"/>
-      <c r="I28" s="29"/>
-      <c r="J28" s="30"/>
-      <c r="K28" s="28"/>
-      <c r="L28" s="29"/>
-      <c r="M28" s="29"/>
-      <c r="N28" s="29"/>
-      <c r="O28" s="29"/>
-      <c r="P28" s="29"/>
-      <c r="Q28" s="30"/>
+      <c r="B28" s="76"/>
+      <c r="C28" s="72"/>
+      <c r="D28" s="72"/>
+      <c r="E28" s="72"/>
+      <c r="F28" s="72"/>
+      <c r="G28" s="78"/>
+      <c r="H28" s="76"/>
+      <c r="I28" s="72"/>
+      <c r="J28" s="78"/>
+      <c r="K28" s="76"/>
+      <c r="L28" s="72"/>
+      <c r="M28" s="72"/>
+      <c r="N28" s="72"/>
+      <c r="O28" s="72"/>
+      <c r="P28" s="72"/>
+      <c r="Q28" s="78"/>
       <c r="R28" s="1"/>
     </row>
     <row r="29" spans="1:18" ht="0.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="1"/>
-      <c r="B29" s="28"/>
-      <c r="C29" s="29"/>
-      <c r="D29" s="29"/>
-      <c r="E29" s="29"/>
-      <c r="F29" s="29"/>
-      <c r="G29" s="30"/>
-      <c r="H29" s="28"/>
-      <c r="I29" s="29"/>
-      <c r="J29" s="30"/>
-      <c r="K29" s="31"/>
-      <c r="L29" s="32"/>
-      <c r="M29" s="32"/>
-      <c r="N29" s="32"/>
-      <c r="O29" s="32"/>
-      <c r="P29" s="32"/>
-      <c r="Q29" s="33"/>
+      <c r="B29" s="76"/>
+      <c r="C29" s="72"/>
+      <c r="D29" s="72"/>
+      <c r="E29" s="72"/>
+      <c r="F29" s="72"/>
+      <c r="G29" s="78"/>
+      <c r="H29" s="76"/>
+      <c r="I29" s="72"/>
+      <c r="J29" s="78"/>
+      <c r="K29" s="27"/>
+      <c r="L29" s="28"/>
+      <c r="M29" s="28"/>
+      <c r="N29" s="28"/>
+      <c r="O29" s="28"/>
+      <c r="P29" s="28"/>
+      <c r="Q29" s="38"/>
       <c r="R29" s="1"/>
     </row>
     <row r="30" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="1"/>
-      <c r="B30" s="31"/>
-      <c r="C30" s="32"/>
-      <c r="D30" s="32"/>
-      <c r="E30" s="32"/>
-      <c r="F30" s="32"/>
-      <c r="G30" s="33"/>
-      <c r="H30" s="31"/>
-      <c r="I30" s="32"/>
-      <c r="J30" s="33"/>
-      <c r="K30" s="34" t="s">
+      <c r="B30" s="27"/>
+      <c r="C30" s="28"/>
+      <c r="D30" s="28"/>
+      <c r="E30" s="28"/>
+      <c r="F30" s="28"/>
+      <c r="G30" s="38"/>
+      <c r="H30" s="27"/>
+      <c r="I30" s="28"/>
+      <c r="J30" s="38"/>
+      <c r="K30" s="61" t="s">
         <v>52</v>
       </c>
-      <c r="L30" s="32"/>
-      <c r="M30" s="32"/>
-      <c r="N30" s="32"/>
-      <c r="O30" s="32"/>
-      <c r="P30" s="32"/>
-      <c r="Q30" s="33"/>
+      <c r="L30" s="28"/>
+      <c r="M30" s="28"/>
+      <c r="N30" s="28"/>
+      <c r="O30" s="28"/>
+      <c r="P30" s="28"/>
+      <c r="Q30" s="38"/>
       <c r="R30" s="1"/>
     </row>
     <row r="31" spans="1:18" ht="3.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2282,24 +2415,24 @@
       <c r="R31" s="1"/>
     </row>
     <row r="32" spans="1:18" ht="19" x14ac:dyDescent="0.2">
-      <c r="B32" s="35" t="s">
+      <c r="B32" s="80" t="s">
         <v>53</v>
       </c>
-      <c r="C32" s="29"/>
-      <c r="D32" s="29"/>
-      <c r="E32" s="29"/>
-      <c r="F32" s="29"/>
-      <c r="G32" s="29"/>
-      <c r="H32" s="29"/>
-      <c r="I32" s="29"/>
-      <c r="J32" s="29"/>
-      <c r="K32" s="29"/>
-      <c r="L32" s="29"/>
-      <c r="M32" s="29"/>
-      <c r="N32" s="29"/>
-      <c r="O32" s="29"/>
-      <c r="P32" s="29"/>
-      <c r="Q32" s="29"/>
+      <c r="C32" s="72"/>
+      <c r="D32" s="72"/>
+      <c r="E32" s="72"/>
+      <c r="F32" s="72"/>
+      <c r="G32" s="72"/>
+      <c r="H32" s="72"/>
+      <c r="I32" s="72"/>
+      <c r="J32" s="72"/>
+      <c r="K32" s="72"/>
+      <c r="L32" s="72"/>
+      <c r="M32" s="72"/>
+      <c r="N32" s="72"/>
+      <c r="O32" s="72"/>
+      <c r="P32" s="72"/>
+      <c r="Q32" s="72"/>
     </row>
     <row r="33" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="34" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3271,19 +3404,32 @@
     <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="55">
-    <mergeCell ref="B10:H10"/>
-    <mergeCell ref="B11:Q11"/>
-    <mergeCell ref="B16:G17"/>
-    <mergeCell ref="B15:H15"/>
-    <mergeCell ref="K16:L17"/>
-    <mergeCell ref="P15:Q15"/>
-    <mergeCell ref="P16:Q17"/>
-    <mergeCell ref="J16:J17"/>
-    <mergeCell ref="B12:Q12"/>
-    <mergeCell ref="I15:O15"/>
-    <mergeCell ref="B13:Q14"/>
-    <mergeCell ref="H16:H17"/>
-    <mergeCell ref="I16:I17"/>
+    <mergeCell ref="B23:G23"/>
+    <mergeCell ref="B24:G24"/>
+    <mergeCell ref="K26:Q29"/>
+    <mergeCell ref="K30:Q30"/>
+    <mergeCell ref="B32:Q32"/>
+    <mergeCell ref="B27:G30"/>
+    <mergeCell ref="B26:G26"/>
+    <mergeCell ref="H23:J30"/>
+    <mergeCell ref="B25:G25"/>
+    <mergeCell ref="P23:Q23"/>
+    <mergeCell ref="K24:Q25"/>
+    <mergeCell ref="K23:O23"/>
+    <mergeCell ref="P18:Q18"/>
+    <mergeCell ref="N18:O18"/>
+    <mergeCell ref="B18:G18"/>
+    <mergeCell ref="P19:Q19"/>
+    <mergeCell ref="N19:O19"/>
+    <mergeCell ref="B19:G19"/>
+    <mergeCell ref="K19:L19"/>
+    <mergeCell ref="K18:L18"/>
+    <mergeCell ref="F3:N3"/>
+    <mergeCell ref="B2:Q2"/>
+    <mergeCell ref="G5:M5"/>
+    <mergeCell ref="B3:C4"/>
+    <mergeCell ref="O3:Q4"/>
+    <mergeCell ref="G4:M4"/>
     <mergeCell ref="B8:I8"/>
     <mergeCell ref="J8:Q8"/>
     <mergeCell ref="B6:Q7"/>
@@ -3300,37 +3446,23 @@
     <mergeCell ref="M16:O16"/>
     <mergeCell ref="N17:O17"/>
     <mergeCell ref="B9:I9"/>
-    <mergeCell ref="F3:N3"/>
-    <mergeCell ref="B2:Q2"/>
-    <mergeCell ref="G5:M5"/>
-    <mergeCell ref="B3:C4"/>
-    <mergeCell ref="O3:Q4"/>
-    <mergeCell ref="G4:M4"/>
-    <mergeCell ref="P18:Q18"/>
-    <mergeCell ref="N18:O18"/>
-    <mergeCell ref="B18:G18"/>
-    <mergeCell ref="P19:Q19"/>
-    <mergeCell ref="N19:O19"/>
-    <mergeCell ref="B19:G19"/>
-    <mergeCell ref="K19:L19"/>
-    <mergeCell ref="K18:L18"/>
-    <mergeCell ref="B23:G23"/>
-    <mergeCell ref="B24:G24"/>
-    <mergeCell ref="K26:Q29"/>
-    <mergeCell ref="K30:Q30"/>
-    <mergeCell ref="B32:Q32"/>
-    <mergeCell ref="B27:G30"/>
-    <mergeCell ref="B26:G26"/>
-    <mergeCell ref="H23:J30"/>
-    <mergeCell ref="B25:G25"/>
-    <mergeCell ref="P23:Q23"/>
-    <mergeCell ref="K24:Q25"/>
-    <mergeCell ref="K23:O23"/>
+    <mergeCell ref="B10:H10"/>
+    <mergeCell ref="B11:Q11"/>
+    <mergeCell ref="B16:G17"/>
+    <mergeCell ref="B15:H15"/>
+    <mergeCell ref="K16:L17"/>
+    <mergeCell ref="P15:Q15"/>
+    <mergeCell ref="P16:Q17"/>
+    <mergeCell ref="J16:J17"/>
+    <mergeCell ref="B12:Q12"/>
+    <mergeCell ref="I15:O15"/>
+    <mergeCell ref="B13:Q14"/>
+    <mergeCell ref="H16:H17"/>
+    <mergeCell ref="I16:I17"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageSetup paperSize="9" scale="98" fitToHeight="100" orientation="portrait"/>
   <drawing r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
CRM-2783 Change address on all Invoice's template
</commit_message>
<xml_diff>
--- a/application/controllers/excel-templates/247around_Tax_Invoice_Inter_State.xlsx
+++ b/application/controllers/excel-templates/247around_Tax_Invoice_Inter_State.xlsx
@@ -1,12 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\247around-adminp-aws\application\controllers\excel-templates\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD7E1405-BBB9-421F-BBA7-52FAEEBCC3CD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Tax Invoice - Inter State" sheetId="1" r:id="rId3"/>
+    <sheet name="Tax Invoice - Inter State" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -16,9 +33,6 @@
     <t>Blackmelon Advance Technology Co. Pvt. Ltd.</t>
   </si>
   <si>
-    <t>A-1/7a, A BLOCK, KRISHNA NAGAR, DELHI 110051</t>
-  </si>
-  <si>
     <t>({meta:recipient_type})</t>
   </si>
   <si>
@@ -174,67 +188,73 @@
   </si>
   <si>
     <t>This is a computer generated invoice, no signature is required.</t>
+  </si>
+  <si>
+    <t>A-1/7, F/F A BLOCK, KRISHNA NAGAR, Delhi, 110051</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="11">
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
       <b/>
-      <sz val="18.0"/>
+      <sz val="18"/>
       <color rgb="FF000000"/>
       <name val="Bookman Old Style"/>
     </font>
-    <font/>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
     <font>
       <b/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
       <b/>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Bookman Old Style"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Bookman Old Style"/>
     </font>
     <font>
       <b/>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Bookman Old Style"/>
     </font>
     <font>
-      <sz val="14.0"/>
+      <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
       <b/>
-      <sz val="14.0"/>
+      <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
       <b/>
-      <sz val="14.0"/>
+      <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="Bookman Old Style"/>
     </font>
@@ -244,7 +264,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -254,79 +274,119 @@
     </fill>
   </fills>
   <borders count="53">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left style="medium">
         <color rgb="FF000000"/>
       </left>
+      <right/>
       <top style="medium">
         <color rgb="FF000000"/>
       </top>
-    </border>
-    <border>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="medium">
         <color rgb="FF000000"/>
       </top>
-    </border>
-    <border>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="medium">
         <color rgb="FF000000"/>
       </right>
       <top style="medium">
         <color rgb="FF000000"/>
       </top>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="medium">
         <color rgb="FF000000"/>
       </left>
-    </border>
-    <border>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="medium">
         <color rgb="FF000000"/>
       </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="medium">
         <color rgb="FF000000"/>
       </left>
+      <right/>
+      <top/>
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
-    </border>
-    <border>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
-    </border>
-    <border>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="medium">
         <color rgb="FF000000"/>
       </right>
+      <top/>
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="medium">
         <color rgb="FF000000"/>
       </left>
+      <right/>
       <top style="medium">
         <color rgb="FF000000"/>
       </top>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
-    </border>
-    <border>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="medium">
         <color rgb="FF000000"/>
       </top>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
-    </border>
-    <border>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="medium">
         <color rgb="FF000000"/>
       </right>
@@ -336,27 +396,34 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="medium">
         <color rgb="FF000000"/>
       </left>
+      <right/>
       <top style="medium">
         <color rgb="FF000000"/>
       </top>
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
-    </border>
-    <border>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="medium">
         <color rgb="FF000000"/>
       </top>
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
-    </border>
-    <border>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="medium">
         <color rgb="FF000000"/>
       </right>
@@ -366,27 +433,34 @@
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="medium">
         <color rgb="FF000000"/>
       </left>
+      <right/>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
-    </border>
-    <border>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
-    </border>
-    <border>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="medium">
         <color rgb="FF000000"/>
       </right>
@@ -396,6 +470,7 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -410,72 +485,102 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="medium">
         <color rgb="FF000000"/>
       </left>
+      <right/>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
-    </border>
-    <border>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
-    </border>
-    <border>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="medium">
         <color rgb="FF000000"/>
       </right>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="medium">
         <color rgb="FF000000"/>
       </left>
+      <right/>
+      <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
-    </border>
-    <border>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
-    </border>
-    <border>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="medium">
         <color rgb="FF000000"/>
       </right>
+      <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
-    </border>
-    <border>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
+      <right/>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
-    </border>
-    <border>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
       <top style="medium">
         <color rgb="FF000000"/>
       </top>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -487,27 +592,35 @@
       <top style="medium">
         <color rgb="FF000000"/>
       </top>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
+      <right/>
       <top style="medium">
         <color rgb="FF000000"/>
       </top>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
+      <right/>
       <top style="medium">
         <color rgb="FF000000"/>
       </top>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
-    </border>
-    <border>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
@@ -517,14 +630,18 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
-    </border>
-    <border>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
+      <top/>
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -533,17 +650,22 @@
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
+      <top/>
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
+      <right/>
+      <top/>
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -558,19 +680,23 @@
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
+      <right/>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
-    </border>
-    <border>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
@@ -580,11 +706,16 @@
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
-    </border>
-    <border>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -593,8 +724,12 @@
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
-    </border>
-    <border>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
@@ -604,6 +739,7 @@
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -618,16 +754,21 @@
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
-    </border>
-    <border>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
+      <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
-    </border>
-    <border>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
@@ -637,27 +778,34 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="medium">
         <color rgb="FF000000"/>
       </left>
+      <right/>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
-    </border>
-    <border>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
-    </border>
-    <border>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="medium">
         <color rgb="FF000000"/>
       </right>
@@ -667,275 +815,304 @@
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="medium">
         <color rgb="FF000000"/>
       </left>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom/>
-    </border>
-    <border>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom/>
-    </border>
-    <border>
       <right/>
       <top style="medium">
         <color rgb="FF000000"/>
       </top>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="medium">
         <color rgb="FF000000"/>
       </left>
+      <right/>
+      <top/>
       <bottom/>
-    </border>
-    <border>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom/>
-    </border>
-    <border>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="medium">
         <color rgb="FF000000"/>
       </right>
+      <top/>
       <bottom/>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="96">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+  <cellXfs count="98">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="3" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="4" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="5" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="4" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="6" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="7" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="7" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf borderId="7" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="7" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="7" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf borderId="8" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="6" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="8" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="9" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf borderId="10" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="11" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="12" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf borderId="13" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="14" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="15" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf borderId="16" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="17" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="10" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf borderId="18" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="12" fillId="2" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="19" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="20" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="21" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="22" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="23" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="24" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="19" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf borderId="20" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf borderId="25" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="26" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="9" fillId="0" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="27" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="28" fillId="2" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="28" fillId="2" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="29" fillId="2" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="30" fillId="2" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="31" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="29" fillId="2" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="32" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="33" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="34" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="35" fillId="2" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="36" fillId="2" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="37" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="4" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="38" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="39" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="38" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="12" fillId="2" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="40" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="41" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf borderId="41" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="13" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="6" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="22" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf borderId="42" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="22" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="15" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf borderId="43" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="15" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="44" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf borderId="45" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="44" fillId="0" fontId="9" numFmtId="1" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="46" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="47" fillId="2" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="48" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="49" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="13" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf borderId="12" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="1" fillId="2" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="44" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf borderId="50" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="51" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="52" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
@@ -946,11 +1123,17 @@
     <xdr:ext cx="533400" cy="619125"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image1.png" title="Image"/>
+        <xdr:cNvPr id="2" name="image1.png" title="Image">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip cstate="print" r:embed="rId1"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -974,11 +1157,17 @@
     <xdr:ext cx="1133475" cy="1095375"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image2.jpg" title="Image"/>
+        <xdr:cNvPr id="3" name="image2.jpg" title="Image">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip cstate="print" r:embed="rId2"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1002,11 +1191,17 @@
     <xdr:ext cx="1190625" cy="342900"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image3.png" title="Image"/>
+        <xdr:cNvPr id="4" name="image3.png" title="Image">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip cstate="print" r:embed="rId3"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1030,11 +1225,17 @@
     <xdr:ext cx="523875" cy="628650"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image4.png"/>
+        <xdr:cNvPr id="5" name="image4.png">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip cstate="print" r:embed="rId4"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4" cstate="print"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1058,11 +1259,17 @@
     <xdr:ext cx="523875" cy="628650"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image4.png"/>
+        <xdr:cNvPr id="6" name="image4.png">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip cstate="print" r:embed="rId4"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4" cstate="print"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1079,37 +1286,332 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:R1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="X13" sqref="X13"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="0.86"/>
-    <col customWidth="1" min="2" max="2" width="2.71"/>
-    <col customWidth="1" min="3" max="3" width="7.29"/>
-    <col customWidth="1" min="4" max="4" width="4.14"/>
-    <col customWidth="1" min="5" max="5" width="5.29"/>
-    <col customWidth="1" min="6" max="6" width="3.71"/>
-    <col customWidth="1" min="7" max="7" width="6.14"/>
-    <col customWidth="1" min="8" max="8" width="9.71"/>
-    <col customWidth="1" min="9" max="9" width="6.14"/>
-    <col customWidth="1" min="10" max="10" width="10.0"/>
-    <col customWidth="1" min="11" max="11" width="1.14"/>
-    <col customWidth="1" min="12" max="12" width="9.86"/>
-    <col customWidth="1" min="13" max="13" width="5.14"/>
-    <col customWidth="1" min="14" max="14" width="4.29"/>
-    <col customWidth="1" min="15" max="15" width="6.14"/>
-    <col customWidth="1" min="16" max="16" width="5.43"/>
-    <col customWidth="1" min="17" max="17" width="8.71"/>
-    <col customWidth="1" min="18" max="18" width="0.86"/>
+    <col min="1" max="1" width="0.88671875" customWidth="1"/>
+    <col min="2" max="2" width="2.6640625" customWidth="1"/>
+    <col min="3" max="3" width="7.33203125" customWidth="1"/>
+    <col min="4" max="4" width="4.109375" customWidth="1"/>
+    <col min="5" max="5" width="5.33203125" customWidth="1"/>
+    <col min="6" max="6" width="3.6640625" customWidth="1"/>
+    <col min="7" max="7" width="6.109375" customWidth="1"/>
+    <col min="8" max="8" width="9.6640625" customWidth="1"/>
+    <col min="9" max="9" width="6.109375" customWidth="1"/>
+    <col min="10" max="10" width="10" customWidth="1"/>
+    <col min="11" max="11" width="1.109375" customWidth="1"/>
+    <col min="12" max="12" width="9.88671875" customWidth="1"/>
+    <col min="13" max="13" width="5.109375" customWidth="1"/>
+    <col min="14" max="14" width="4.33203125" customWidth="1"/>
+    <col min="15" max="15" width="6.109375" customWidth="1"/>
+    <col min="16" max="16" width="5.44140625" customWidth="1"/>
+    <col min="17" max="17" width="8.6640625" customWidth="1"/>
+    <col min="18" max="18" width="0.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="3.75" customHeight="1">
+    <row r="1" spans="1:18" ht="3.75" customHeight="1">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -1129,133 +1631,152 @@
       <c r="Q1" s="1"/>
       <c r="R1" s="1"/>
     </row>
-    <row r="2" ht="29.25" customHeight="1">
+    <row r="2" spans="1:18" ht="29.25" customHeight="1">
       <c r="A2" s="1"/>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="93" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
-      <c r="M2" s="3"/>
-      <c r="N2" s="3"/>
-      <c r="O2" s="3"/>
-      <c r="P2" s="3"/>
-      <c r="Q2" s="4"/>
+      <c r="C2" s="53"/>
+      <c r="D2" s="53"/>
+      <c r="E2" s="53"/>
+      <c r="F2" s="53"/>
+      <c r="G2" s="53"/>
+      <c r="H2" s="53"/>
+      <c r="I2" s="53"/>
+      <c r="J2" s="53"/>
+      <c r="K2" s="53"/>
+      <c r="L2" s="53"/>
+      <c r="M2" s="53"/>
+      <c r="N2" s="53"/>
+      <c r="O2" s="53"/>
+      <c r="P2" s="53"/>
+      <c r="Q2" s="42"/>
       <c r="R2" s="1"/>
     </row>
-    <row r="3" ht="30.0" customHeight="1">
+    <row r="3" spans="1:18" ht="30" customHeight="1">
       <c r="A3" s="1"/>
-      <c r="B3" s="5"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="7" t="s">
+      <c r="B3" s="94"/>
+      <c r="C3" s="62"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="82" t="s">
+        <v>53</v>
+      </c>
+      <c r="G3" s="62"/>
+      <c r="H3" s="62"/>
+      <c r="I3" s="62"/>
+      <c r="J3" s="62"/>
+      <c r="K3" s="62"/>
+      <c r="L3" s="62"/>
+      <c r="M3" s="62"/>
+      <c r="N3" s="62"/>
+      <c r="O3" s="83" t="s">
         <v>1</v>
       </c>
-      <c r="O3" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q3" s="9"/>
+      <c r="P3" s="62"/>
+      <c r="Q3" s="49"/>
       <c r="R3" s="1"/>
     </row>
-    <row r="4">
+    <row r="4" spans="1:18" ht="15.6">
       <c r="A4" s="1"/>
-      <c r="B4" s="10"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="N4" s="13"/>
-      <c r="Q4" s="9"/>
+      <c r="B4" s="64"/>
+      <c r="C4" s="62"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="90" t="s">
+        <v>2</v>
+      </c>
+      <c r="H4" s="62"/>
+      <c r="I4" s="62"/>
+      <c r="J4" s="62"/>
+      <c r="K4" s="62"/>
+      <c r="L4" s="62"/>
+      <c r="M4" s="62"/>
+      <c r="N4" s="5"/>
+      <c r="O4" s="62"/>
+      <c r="P4" s="62"/>
+      <c r="Q4" s="49"/>
       <c r="R4" s="1"/>
     </row>
-    <row r="5">
+    <row r="5" spans="1:18" ht="15.6">
       <c r="A5" s="1"/>
-      <c r="B5" s="14"/>
-      <c r="C5" s="15"/>
-      <c r="D5" s="16"/>
-      <c r="E5" s="16"/>
-      <c r="F5" s="16"/>
-      <c r="G5" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="H5" s="18"/>
-      <c r="I5" s="18"/>
-      <c r="J5" s="18"/>
-      <c r="K5" s="18"/>
-      <c r="L5" s="18"/>
-      <c r="M5" s="18"/>
-      <c r="N5" s="17"/>
-      <c r="O5" s="17"/>
-      <c r="P5" s="19"/>
-      <c r="Q5" s="20"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="89" t="s">
+        <v>3</v>
+      </c>
+      <c r="H5" s="55"/>
+      <c r="I5" s="55"/>
+      <c r="J5" s="55"/>
+      <c r="K5" s="55"/>
+      <c r="L5" s="55"/>
+      <c r="M5" s="55"/>
+      <c r="N5" s="9"/>
+      <c r="O5" s="9"/>
+      <c r="P5" s="10"/>
+      <c r="Q5" s="11"/>
       <c r="R5" s="1"/>
     </row>
-    <row r="6" ht="15.75" customHeight="1">
+    <row r="6" spans="1:18" ht="15.75" customHeight="1">
       <c r="A6" s="1"/>
-      <c r="B6" s="21" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
-      <c r="L6" s="3"/>
-      <c r="M6" s="3"/>
-      <c r="N6" s="3"/>
-      <c r="O6" s="3"/>
-      <c r="P6" s="3"/>
-      <c r="Q6" s="4"/>
+      <c r="B6" s="92" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="53"/>
+      <c r="D6" s="53"/>
+      <c r="E6" s="53"/>
+      <c r="F6" s="53"/>
+      <c r="G6" s="53"/>
+      <c r="H6" s="53"/>
+      <c r="I6" s="53"/>
+      <c r="J6" s="53"/>
+      <c r="K6" s="53"/>
+      <c r="L6" s="53"/>
+      <c r="M6" s="53"/>
+      <c r="N6" s="53"/>
+      <c r="O6" s="53"/>
+      <c r="P6" s="53"/>
+      <c r="Q6" s="42"/>
       <c r="R6" s="1"/>
     </row>
-    <row r="7" ht="7.5" customHeight="1">
+    <row r="7" spans="1:18" ht="7.5" customHeight="1">
       <c r="A7" s="1"/>
-      <c r="B7" s="22"/>
-      <c r="C7" s="18"/>
-      <c r="D7" s="18"/>
-      <c r="E7" s="18"/>
-      <c r="F7" s="18"/>
-      <c r="G7" s="18"/>
-      <c r="H7" s="18"/>
-      <c r="I7" s="18"/>
-      <c r="J7" s="18"/>
-      <c r="K7" s="18"/>
-      <c r="L7" s="18"/>
-      <c r="M7" s="18"/>
-      <c r="N7" s="18"/>
-      <c r="O7" s="18"/>
-      <c r="P7" s="18"/>
-      <c r="Q7" s="23"/>
+      <c r="B7" s="54"/>
+      <c r="C7" s="55"/>
+      <c r="D7" s="55"/>
+      <c r="E7" s="55"/>
+      <c r="F7" s="55"/>
+      <c r="G7" s="55"/>
+      <c r="H7" s="55"/>
+      <c r="I7" s="55"/>
+      <c r="J7" s="55"/>
+      <c r="K7" s="55"/>
+      <c r="L7" s="55"/>
+      <c r="M7" s="55"/>
+      <c r="N7" s="55"/>
+      <c r="O7" s="55"/>
+      <c r="P7" s="55"/>
+      <c r="Q7" s="43"/>
       <c r="R7" s="1"/>
     </row>
-    <row r="8" ht="21.75" customHeight="1">
+    <row r="8" spans="1:18" ht="21.75" customHeight="1">
       <c r="A8" s="1"/>
-      <c r="B8" s="24" t="s">
+      <c r="B8" s="30" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="31"/>
+      <c r="D8" s="31"/>
+      <c r="E8" s="31"/>
+      <c r="F8" s="31"/>
+      <c r="G8" s="31"/>
+      <c r="H8" s="31"/>
+      <c r="I8" s="32"/>
+      <c r="J8" s="91" t="s">
         <v>6</v>
-      </c>
-      <c r="C8" s="25"/>
-      <c r="D8" s="25"/>
-      <c r="E8" s="25"/>
-      <c r="F8" s="25"/>
-      <c r="G8" s="25"/>
-      <c r="H8" s="25"/>
-      <c r="I8" s="26"/>
-      <c r="J8" s="27" t="s">
-        <v>7</v>
       </c>
       <c r="K8" s="28"/>
       <c r="L8" s="28"/>
@@ -1266,58 +1787,58 @@
       <c r="Q8" s="29"/>
       <c r="R8" s="1"/>
     </row>
-    <row r="9" ht="21.0" customHeight="1">
+    <row r="9" spans="1:18" ht="21" customHeight="1">
       <c r="A9" s="1"/>
-      <c r="B9" s="30" t="s">
+      <c r="B9" s="50" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="51"/>
+      <c r="D9" s="51"/>
+      <c r="E9" s="51"/>
+      <c r="F9" s="51"/>
+      <c r="G9" s="51"/>
+      <c r="H9" s="51"/>
+      <c r="I9" s="88"/>
+      <c r="J9" s="60" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="31"/>
-      <c r="D9" s="31"/>
-      <c r="E9" s="31"/>
-      <c r="F9" s="31"/>
-      <c r="G9" s="31"/>
-      <c r="H9" s="31"/>
-      <c r="I9" s="32"/>
-      <c r="J9" s="33" t="s">
-        <v>9</v>
-      </c>
-      <c r="K9" s="25"/>
-      <c r="L9" s="25"/>
-      <c r="M9" s="25"/>
-      <c r="N9" s="25"/>
-      <c r="O9" s="25"/>
-      <c r="P9" s="25"/>
-      <c r="Q9" s="26"/>
+      <c r="K9" s="31"/>
+      <c r="L9" s="31"/>
+      <c r="M9" s="31"/>
+      <c r="N9" s="31"/>
+      <c r="O9" s="31"/>
+      <c r="P9" s="31"/>
+      <c r="Q9" s="32"/>
       <c r="R9" s="1"/>
     </row>
-    <row r="10" ht="19.5" customHeight="1">
+    <row r="10" spans="1:18" ht="19.5" customHeight="1">
       <c r="A10" s="1"/>
-      <c r="B10" s="30" t="s">
+      <c r="B10" s="50" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="51"/>
+      <c r="D10" s="51"/>
+      <c r="E10" s="51"/>
+      <c r="F10" s="51"/>
+      <c r="G10" s="51"/>
+      <c r="H10" s="51"/>
+      <c r="I10" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="31"/>
-      <c r="D10" s="31"/>
-      <c r="E10" s="31"/>
-      <c r="F10" s="31"/>
-      <c r="G10" s="31"/>
-      <c r="H10" s="31"/>
-      <c r="I10" s="34" t="s">
-        <v>11</v>
-      </c>
-      <c r="J10" s="33"/>
-      <c r="K10" s="25"/>
-      <c r="L10" s="25"/>
-      <c r="M10" s="25"/>
-      <c r="N10" s="25"/>
-      <c r="O10" s="25"/>
-      <c r="P10" s="25"/>
-      <c r="Q10" s="26"/>
+      <c r="J10" s="60"/>
+      <c r="K10" s="31"/>
+      <c r="L10" s="31"/>
+      <c r="M10" s="31"/>
+      <c r="N10" s="31"/>
+      <c r="O10" s="31"/>
+      <c r="P10" s="31"/>
+      <c r="Q10" s="32"/>
       <c r="R10" s="1"/>
     </row>
-    <row r="11">
+    <row r="11" spans="1:18" ht="18">
       <c r="A11" s="1"/>
-      <c r="B11" s="35" t="s">
-        <v>12</v>
+      <c r="B11" s="27" t="s">
+        <v>11</v>
       </c>
       <c r="C11" s="28"/>
       <c r="D11" s="28"/>
@@ -1336,469 +1857,512 @@
       <c r="Q11" s="29"/>
       <c r="R11" s="1"/>
     </row>
-    <row r="12" ht="24.75" customHeight="1">
+    <row r="12" spans="1:18" ht="24.75" customHeight="1">
       <c r="A12" s="1"/>
-      <c r="B12" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="C12" s="25"/>
-      <c r="D12" s="25"/>
-      <c r="E12" s="25"/>
-      <c r="F12" s="25"/>
-      <c r="G12" s="25"/>
-      <c r="H12" s="25"/>
-      <c r="I12" s="25"/>
-      <c r="J12" s="25"/>
-      <c r="K12" s="25"/>
-      <c r="L12" s="25"/>
-      <c r="M12" s="25"/>
-      <c r="N12" s="25"/>
-      <c r="O12" s="25"/>
-      <c r="P12" s="25"/>
-      <c r="Q12" s="26"/>
+      <c r="B12" s="30" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="31"/>
+      <c r="D12" s="31"/>
+      <c r="E12" s="31"/>
+      <c r="F12" s="31"/>
+      <c r="G12" s="31"/>
+      <c r="H12" s="31"/>
+      <c r="I12" s="31"/>
+      <c r="J12" s="31"/>
+      <c r="K12" s="31"/>
+      <c r="L12" s="31"/>
+      <c r="M12" s="31"/>
+      <c r="N12" s="31"/>
+      <c r="O12" s="31"/>
+      <c r="P12" s="31"/>
+      <c r="Q12" s="32"/>
       <c r="R12" s="1"/>
     </row>
-    <row r="13">
+    <row r="13" spans="1:18" ht="14.4">
       <c r="A13" s="1"/>
       <c r="B13" s="36" t="s">
-        <v>14</v>
-      </c>
-      <c r="C13" s="37"/>
-      <c r="D13" s="37"/>
-      <c r="E13" s="37"/>
-      <c r="F13" s="37"/>
-      <c r="G13" s="37"/>
-      <c r="H13" s="37"/>
-      <c r="I13" s="37"/>
-      <c r="J13" s="37"/>
-      <c r="K13" s="37"/>
-      <c r="L13" s="37"/>
-      <c r="M13" s="37"/>
-      <c r="N13" s="37"/>
-      <c r="O13" s="37"/>
-      <c r="P13" s="37"/>
-      <c r="Q13" s="38"/>
+        <v>13</v>
+      </c>
+      <c r="C13" s="34"/>
+      <c r="D13" s="34"/>
+      <c r="E13" s="34"/>
+      <c r="F13" s="34"/>
+      <c r="G13" s="34"/>
+      <c r="H13" s="34"/>
+      <c r="I13" s="34"/>
+      <c r="J13" s="34"/>
+      <c r="K13" s="34"/>
+      <c r="L13" s="34"/>
+      <c r="M13" s="34"/>
+      <c r="N13" s="34"/>
+      <c r="O13" s="34"/>
+      <c r="P13" s="34"/>
+      <c r="Q13" s="37"/>
       <c r="R13" s="1"/>
     </row>
-    <row r="14" ht="15.75" customHeight="1">
+    <row r="14" spans="1:18" ht="15.75" customHeight="1">
       <c r="A14" s="1"/>
-      <c r="B14" s="39"/>
-      <c r="C14" s="40"/>
-      <c r="D14" s="40"/>
-      <c r="E14" s="40"/>
-      <c r="F14" s="40"/>
-      <c r="G14" s="40"/>
-      <c r="H14" s="40"/>
-      <c r="I14" s="40"/>
-      <c r="J14" s="40"/>
-      <c r="K14" s="40"/>
-      <c r="L14" s="40"/>
-      <c r="M14" s="40"/>
-      <c r="N14" s="40"/>
-      <c r="O14" s="40"/>
-      <c r="P14" s="40"/>
-      <c r="Q14" s="41"/>
+      <c r="B14" s="38"/>
+      <c r="C14" s="39"/>
+      <c r="D14" s="39"/>
+      <c r="E14" s="39"/>
+      <c r="F14" s="39"/>
+      <c r="G14" s="39"/>
+      <c r="H14" s="39"/>
+      <c r="I14" s="39"/>
+      <c r="J14" s="39"/>
+      <c r="K14" s="39"/>
+      <c r="L14" s="39"/>
+      <c r="M14" s="39"/>
+      <c r="N14" s="39"/>
+      <c r="O14" s="39"/>
+      <c r="P14" s="39"/>
+      <c r="Q14" s="40"/>
       <c r="R14" s="1"/>
     </row>
-    <row r="15" ht="25.5" customHeight="1">
+    <row r="15" spans="1:18" ht="25.5" customHeight="1">
       <c r="A15" s="1"/>
-      <c r="B15" s="42" t="s">
+      <c r="B15" s="56" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" s="34"/>
+      <c r="D15" s="34"/>
+      <c r="E15" s="34"/>
+      <c r="F15" s="34"/>
+      <c r="G15" s="34"/>
+      <c r="H15" s="34"/>
+      <c r="I15" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="37"/>
-      <c r="D15" s="37"/>
-      <c r="E15" s="37"/>
-      <c r="F15" s="37"/>
-      <c r="G15" s="37"/>
-      <c r="H15" s="37"/>
-      <c r="I15" s="43" t="s">
+      <c r="J15" s="34"/>
+      <c r="K15" s="34"/>
+      <c r="L15" s="34"/>
+      <c r="M15" s="34"/>
+      <c r="N15" s="34"/>
+      <c r="O15" s="35"/>
+      <c r="P15" s="48" t="s">
         <v>16</v>
       </c>
-      <c r="J15" s="37"/>
-      <c r="K15" s="37"/>
-      <c r="L15" s="37"/>
-      <c r="M15" s="37"/>
-      <c r="N15" s="37"/>
-      <c r="O15" s="44"/>
-      <c r="P15" s="45" t="s">
-        <v>17</v>
-      </c>
-      <c r="Q15" s="38"/>
+      <c r="Q15" s="37"/>
       <c r="R15" s="1"/>
     </row>
-    <row r="16">
+    <row r="16" spans="1:18" ht="18">
       <c r="A16" s="1"/>
-      <c r="B16" s="46" t="s">
+      <c r="B16" s="52" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" s="53"/>
+      <c r="D16" s="53"/>
+      <c r="E16" s="53"/>
+      <c r="F16" s="53"/>
+      <c r="G16" s="20"/>
+      <c r="H16" s="84" t="s">
         <v>18</v>
       </c>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="47"/>
-      <c r="H16" s="48" t="s">
+      <c r="I16" s="57" t="s">
         <v>19</v>
       </c>
-      <c r="I16" s="49" t="s">
+      <c r="J16" s="57" t="s">
         <v>20</v>
       </c>
-      <c r="J16" s="49" t="s">
+      <c r="K16" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="K16" s="50" t="s">
+      <c r="L16" s="20"/>
+      <c r="M16" s="44" t="s">
         <v>22</v>
       </c>
-      <c r="L16" s="47"/>
-      <c r="M16" s="51" t="s">
+      <c r="N16" s="31"/>
+      <c r="O16" s="45"/>
+      <c r="P16" s="41" t="s">
         <v>23</v>
       </c>
-      <c r="N16" s="25"/>
-      <c r="O16" s="52"/>
-      <c r="P16" s="53" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q16" s="4"/>
+      <c r="Q16" s="42"/>
       <c r="R16" s="1"/>
     </row>
-    <row r="17" ht="25.5" customHeight="1">
+    <row r="17" spans="1:18" ht="25.5" customHeight="1">
       <c r="A17" s="1"/>
-      <c r="B17" s="22"/>
-      <c r="C17" s="18"/>
-      <c r="D17" s="18"/>
-      <c r="E17" s="18"/>
-      <c r="F17" s="18"/>
-      <c r="G17" s="54"/>
-      <c r="H17" s="55"/>
-      <c r="I17" s="55"/>
-      <c r="J17" s="55"/>
-      <c r="K17" s="56"/>
-      <c r="L17" s="54"/>
-      <c r="M17" s="57" t="s">
-        <v>21</v>
-      </c>
-      <c r="N17" s="58" t="s">
-        <v>25</v>
-      </c>
-      <c r="O17" s="59"/>
-      <c r="P17" s="56"/>
-      <c r="Q17" s="23"/>
+      <c r="B17" s="54"/>
+      <c r="C17" s="55"/>
+      <c r="D17" s="55"/>
+      <c r="E17" s="55"/>
+      <c r="F17" s="55"/>
+      <c r="G17" s="22"/>
+      <c r="H17" s="58"/>
+      <c r="I17" s="58"/>
+      <c r="J17" s="58"/>
+      <c r="K17" s="21"/>
+      <c r="L17" s="22"/>
+      <c r="M17" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="N17" s="46" t="s">
+        <v>24</v>
+      </c>
+      <c r="O17" s="47"/>
+      <c r="P17" s="21"/>
+      <c r="Q17" s="43"/>
       <c r="R17" s="1"/>
     </row>
-    <row r="18" ht="49.5" customHeight="1">
+    <row r="18" spans="1:18" ht="49.5" customHeight="1">
       <c r="A18" s="1"/>
-      <c r="B18" s="60" t="s">
+      <c r="B18" s="61" t="s">
+        <v>25</v>
+      </c>
+      <c r="C18" s="62"/>
+      <c r="D18" s="62"/>
+      <c r="E18" s="62"/>
+      <c r="F18" s="62"/>
+      <c r="G18" s="26"/>
+      <c r="H18" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="G18" s="61"/>
-      <c r="H18" s="62" t="s">
+      <c r="I18" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="I18" s="63" t="s">
+      <c r="J18" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="J18" s="62" t="s">
+      <c r="K18" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="K18" s="64" t="s">
+      <c r="L18" s="26"/>
+      <c r="M18" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="L18" s="61"/>
-      <c r="M18" s="62" t="s">
+      <c r="N18" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="N18" s="64" t="s">
+      <c r="O18" s="26"/>
+      <c r="P18" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="O18" s="61"/>
-      <c r="P18" s="65" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q18" s="9"/>
+      <c r="Q18" s="49"/>
       <c r="R18" s="1"/>
     </row>
-    <row r="19" ht="25.5" customHeight="1">
+    <row r="19" spans="1:18" ht="25.5" customHeight="1">
       <c r="A19" s="1"/>
-      <c r="B19" s="66" t="s">
-        <v>24</v>
+      <c r="B19" s="59" t="s">
+        <v>23</v>
       </c>
       <c r="C19" s="28"/>
       <c r="D19" s="28"/>
       <c r="E19" s="28"/>
       <c r="F19" s="28"/>
-      <c r="G19" s="67"/>
-      <c r="H19" s="68"/>
-      <c r="I19" s="69" t="s">
+      <c r="G19" s="24"/>
+      <c r="H19" s="16"/>
+      <c r="I19" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="J19" s="17"/>
+      <c r="K19" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="J19" s="69"/>
-      <c r="K19" s="70" t="s">
+      <c r="L19" s="24"/>
+      <c r="M19" s="17"/>
+      <c r="N19" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="L19" s="67"/>
-      <c r="M19" s="69"/>
-      <c r="N19" s="70" t="s">
+      <c r="O19" s="24"/>
+      <c r="P19" s="23" t="s">
         <v>36</v>
-      </c>
-      <c r="O19" s="67"/>
-      <c r="P19" s="70" t="s">
-        <v>37</v>
       </c>
       <c r="Q19" s="29"/>
       <c r="R19" s="1"/>
     </row>
-    <row r="20" ht="21.75" customHeight="1">
+    <row r="20" spans="1:18" ht="21.75" customHeight="1">
       <c r="A20" s="1"/>
-      <c r="B20" s="71" t="s">
+      <c r="B20" s="69" t="s">
+        <v>37</v>
+      </c>
+      <c r="C20" s="55"/>
+      <c r="D20" s="55"/>
+      <c r="E20" s="55"/>
+      <c r="F20" s="55"/>
+      <c r="G20" s="55"/>
+      <c r="H20" s="55"/>
+      <c r="I20" s="55"/>
+      <c r="J20" s="55"/>
+      <c r="K20" s="85" t="s">
         <v>38</v>
       </c>
-      <c r="C20" s="18"/>
-      <c r="D20" s="18"/>
-      <c r="E20" s="18"/>
-      <c r="F20" s="18"/>
-      <c r="G20" s="18"/>
-      <c r="H20" s="18"/>
-      <c r="I20" s="18"/>
-      <c r="J20" s="18"/>
-      <c r="K20" s="72" t="s">
+      <c r="L20" s="39"/>
+      <c r="M20" s="39"/>
+      <c r="N20" s="39"/>
+      <c r="O20" s="86"/>
+      <c r="P20" s="87" t="s">
         <v>39</v>
       </c>
-      <c r="L20" s="40"/>
-      <c r="M20" s="40"/>
-      <c r="N20" s="40"/>
-      <c r="O20" s="73"/>
-      <c r="P20" s="74" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q20" s="41"/>
+      <c r="Q20" s="40"/>
       <c r="R20" s="1"/>
     </row>
-    <row r="21" ht="15.75" customHeight="1">
+    <row r="21" spans="1:18" ht="15.75" customHeight="1">
       <c r="A21" s="1"/>
-      <c r="B21" s="75" t="s">
+      <c r="B21" s="73" t="s">
+        <v>40</v>
+      </c>
+      <c r="C21" s="53"/>
+      <c r="D21" s="53"/>
+      <c r="E21" s="53"/>
+      <c r="F21" s="53"/>
+      <c r="G21" s="53"/>
+      <c r="H21" s="53"/>
+      <c r="I21" s="53"/>
+      <c r="J21" s="42"/>
+      <c r="K21" s="96" t="s">
         <v>41</v>
       </c>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
-      <c r="H21" s="3"/>
-      <c r="I21" s="3"/>
-      <c r="J21" s="4"/>
-      <c r="K21" s="76" t="s">
+      <c r="L21" s="51"/>
+      <c r="M21" s="51"/>
+      <c r="N21" s="51"/>
+      <c r="O21" s="97"/>
+      <c r="P21" s="95" t="s">
         <v>42</v>
       </c>
-      <c r="L21" s="31"/>
-      <c r="M21" s="31"/>
-      <c r="N21" s="31"/>
-      <c r="O21" s="77"/>
-      <c r="P21" s="78" t="s">
-        <v>43</v>
-      </c>
-      <c r="Q21" s="32"/>
+      <c r="Q21" s="88"/>
       <c r="R21" s="1"/>
     </row>
-    <row r="22" ht="24.0" customHeight="1">
+    <row r="22" spans="1:18" ht="24" customHeight="1">
       <c r="A22" s="1"/>
-      <c r="B22" s="22"/>
-      <c r="C22" s="18"/>
-      <c r="D22" s="18"/>
-      <c r="E22" s="18"/>
-      <c r="F22" s="18"/>
-      <c r="G22" s="18"/>
-      <c r="H22" s="18"/>
-      <c r="I22" s="18"/>
-      <c r="J22" s="23"/>
-      <c r="K22" s="79" t="s">
+      <c r="B22" s="54"/>
+      <c r="C22" s="55"/>
+      <c r="D22" s="55"/>
+      <c r="E22" s="55"/>
+      <c r="F22" s="55"/>
+      <c r="G22" s="55"/>
+      <c r="H22" s="55"/>
+      <c r="I22" s="55"/>
+      <c r="J22" s="43"/>
+      <c r="K22" s="77" t="s">
+        <v>43</v>
+      </c>
+      <c r="L22" s="78"/>
+      <c r="M22" s="78"/>
+      <c r="N22" s="78"/>
+      <c r="O22" s="47"/>
+      <c r="P22" s="79" t="s">
         <v>44</v>
       </c>
-      <c r="L22" s="80"/>
-      <c r="M22" s="80"/>
-      <c r="N22" s="80"/>
-      <c r="O22" s="59"/>
-      <c r="P22" s="81" t="s">
-        <v>45</v>
-      </c>
-      <c r="Q22" s="82"/>
+      <c r="Q22" s="80"/>
       <c r="R22" s="1"/>
     </row>
-    <row r="23" ht="15.75" customHeight="1">
+    <row r="23" spans="1:18" ht="15.75" customHeight="1">
       <c r="A23" s="1"/>
-      <c r="B23" s="83" t="s">
+      <c r="B23" s="74" t="s">
+        <v>45</v>
+      </c>
+      <c r="C23" s="75"/>
+      <c r="D23" s="75"/>
+      <c r="E23" s="75"/>
+      <c r="F23" s="75"/>
+      <c r="G23" s="76"/>
+      <c r="H23" s="63"/>
+      <c r="I23" s="53"/>
+      <c r="J23" s="42"/>
+      <c r="K23" s="72" t="s">
         <v>46</v>
-      </c>
-      <c r="C23" s="84"/>
-      <c r="D23" s="84"/>
-      <c r="E23" s="84"/>
-      <c r="F23" s="84"/>
-      <c r="G23" s="85"/>
-      <c r="H23" s="86"/>
-      <c r="I23" s="3"/>
-      <c r="J23" s="4"/>
-      <c r="K23" s="87" t="s">
-        <v>47</v>
       </c>
       <c r="L23" s="28"/>
       <c r="M23" s="28"/>
       <c r="N23" s="28"/>
       <c r="O23" s="29"/>
-      <c r="P23" s="88">
+      <c r="P23" s="71">
         <f>IF(I10="Y",P21,0)</f>
         <v>0</v>
       </c>
       <c r="Q23" s="29"/>
       <c r="R23" s="1"/>
     </row>
-    <row r="24" ht="15.75" customHeight="1">
+    <row r="24" spans="1:18" ht="15.75" customHeight="1">
       <c r="A24" s="1"/>
-      <c r="B24" s="24" t="s">
+      <c r="B24" s="30" t="s">
+        <v>47</v>
+      </c>
+      <c r="C24" s="31"/>
+      <c r="D24" s="31"/>
+      <c r="E24" s="31"/>
+      <c r="F24" s="31"/>
+      <c r="G24" s="45"/>
+      <c r="H24" s="64"/>
+      <c r="I24" s="62"/>
+      <c r="J24" s="49"/>
+      <c r="K24" s="65" t="s">
         <v>48</v>
       </c>
-      <c r="C24" s="25"/>
-      <c r="D24" s="25"/>
-      <c r="E24" s="25"/>
-      <c r="F24" s="25"/>
-      <c r="G24" s="52"/>
-      <c r="H24" s="10"/>
-      <c r="J24" s="9"/>
-      <c r="K24" s="89" t="s">
-        <v>49</v>
-      </c>
-      <c r="L24" s="3"/>
-      <c r="M24" s="3"/>
-      <c r="N24" s="3"/>
-      <c r="O24" s="3"/>
-      <c r="P24" s="3"/>
-      <c r="Q24" s="4"/>
+      <c r="L24" s="53"/>
+      <c r="M24" s="53"/>
+      <c r="N24" s="53"/>
+      <c r="O24" s="53"/>
+      <c r="P24" s="53"/>
+      <c r="Q24" s="42"/>
       <c r="R24" s="1"/>
     </row>
-    <row r="25" ht="15.75" customHeight="1">
+    <row r="25" spans="1:18" ht="15.75" customHeight="1">
       <c r="A25" s="1"/>
-      <c r="B25" s="90" t="s">
-        <v>50</v>
-      </c>
-      <c r="C25" s="80"/>
-      <c r="D25" s="80"/>
-      <c r="E25" s="80"/>
-      <c r="F25" s="80"/>
-      <c r="G25" s="59"/>
-      <c r="H25" s="10"/>
-      <c r="J25" s="9"/>
-      <c r="K25" s="91"/>
-      <c r="L25" s="92"/>
-      <c r="M25" s="92"/>
-      <c r="N25" s="92"/>
-      <c r="O25" s="92"/>
-      <c r="P25" s="92"/>
-      <c r="Q25" s="93"/>
+      <c r="B25" s="81" t="s">
+        <v>49</v>
+      </c>
+      <c r="C25" s="78"/>
+      <c r="D25" s="78"/>
+      <c r="E25" s="78"/>
+      <c r="F25" s="78"/>
+      <c r="G25" s="47"/>
+      <c r="H25" s="64"/>
+      <c r="I25" s="62"/>
+      <c r="J25" s="49"/>
+      <c r="K25" s="66"/>
+      <c r="L25" s="67"/>
+      <c r="M25" s="67"/>
+      <c r="N25" s="67"/>
+      <c r="O25" s="67"/>
+      <c r="P25" s="67"/>
+      <c r="Q25" s="68"/>
       <c r="R25" s="1"/>
     </row>
-    <row r="26" ht="15.75" customHeight="1">
+    <row r="26" spans="1:18" ht="15.75" customHeight="1">
       <c r="A26" s="1"/>
-      <c r="B26" s="90" t="s">
-        <v>51</v>
-      </c>
-      <c r="C26" s="80"/>
-      <c r="D26" s="80"/>
-      <c r="E26" s="80"/>
-      <c r="F26" s="80"/>
-      <c r="G26" s="59"/>
-      <c r="H26" s="10"/>
-      <c r="J26" s="9"/>
-      <c r="K26" s="86"/>
-      <c r="L26" s="3"/>
-      <c r="M26" s="3"/>
-      <c r="N26" s="3"/>
-      <c r="O26" s="3"/>
-      <c r="P26" s="3"/>
-      <c r="Q26" s="4"/>
+      <c r="B26" s="81" t="s">
+        <v>50</v>
+      </c>
+      <c r="C26" s="78"/>
+      <c r="D26" s="78"/>
+      <c r="E26" s="78"/>
+      <c r="F26" s="78"/>
+      <c r="G26" s="47"/>
+      <c r="H26" s="64"/>
+      <c r="I26" s="62"/>
+      <c r="J26" s="49"/>
+      <c r="K26" s="63"/>
+      <c r="L26" s="53"/>
+      <c r="M26" s="53"/>
+      <c r="N26" s="53"/>
+      <c r="O26" s="53"/>
+      <c r="P26" s="53"/>
+      <c r="Q26" s="42"/>
       <c r="R26" s="1"/>
     </row>
-    <row r="27" ht="15.75" customHeight="1">
+    <row r="27" spans="1:18" ht="15.75" customHeight="1">
       <c r="A27" s="1"/>
-      <c r="B27" s="94"/>
-      <c r="C27" s="3"/>
-      <c r="D27" s="3"/>
-      <c r="E27" s="3"/>
-      <c r="F27" s="3"/>
-      <c r="G27" s="4"/>
-      <c r="H27" s="10"/>
-      <c r="J27" s="9"/>
-      <c r="K27" s="10"/>
-      <c r="Q27" s="9"/>
+      <c r="B27" s="70"/>
+      <c r="C27" s="53"/>
+      <c r="D27" s="53"/>
+      <c r="E27" s="53"/>
+      <c r="F27" s="53"/>
+      <c r="G27" s="42"/>
+      <c r="H27" s="64"/>
+      <c r="I27" s="62"/>
+      <c r="J27" s="49"/>
+      <c r="K27" s="64"/>
+      <c r="L27" s="62"/>
+      <c r="M27" s="62"/>
+      <c r="N27" s="62"/>
+      <c r="O27" s="62"/>
+      <c r="P27" s="62"/>
+      <c r="Q27" s="49"/>
       <c r="R27" s="1"/>
     </row>
-    <row r="28" ht="3.75" hidden="1" customHeight="1">
+    <row r="28" spans="1:18" ht="3.75" hidden="1" customHeight="1">
       <c r="A28" s="1"/>
-      <c r="B28" s="10"/>
-      <c r="G28" s="9"/>
-      <c r="H28" s="10"/>
-      <c r="J28" s="9"/>
-      <c r="K28" s="10"/>
-      <c r="Q28" s="9"/>
+      <c r="B28" s="64"/>
+      <c r="C28" s="62"/>
+      <c r="D28" s="62"/>
+      <c r="E28" s="62"/>
+      <c r="F28" s="62"/>
+      <c r="G28" s="49"/>
+      <c r="H28" s="64"/>
+      <c r="I28" s="62"/>
+      <c r="J28" s="49"/>
+      <c r="K28" s="64"/>
+      <c r="L28" s="62"/>
+      <c r="M28" s="62"/>
+      <c r="N28" s="62"/>
+      <c r="O28" s="62"/>
+      <c r="P28" s="62"/>
+      <c r="Q28" s="49"/>
       <c r="R28" s="1"/>
     </row>
-    <row r="29" ht="0.75" customHeight="1">
+    <row r="29" spans="1:18" ht="0.75" customHeight="1">
       <c r="A29" s="1"/>
-      <c r="B29" s="10"/>
-      <c r="G29" s="9"/>
-      <c r="H29" s="10"/>
-      <c r="J29" s="9"/>
-      <c r="K29" s="22"/>
-      <c r="L29" s="18"/>
-      <c r="M29" s="18"/>
-      <c r="N29" s="18"/>
-      <c r="O29" s="18"/>
-      <c r="P29" s="18"/>
-      <c r="Q29" s="23"/>
+      <c r="B29" s="64"/>
+      <c r="C29" s="62"/>
+      <c r="D29" s="62"/>
+      <c r="E29" s="62"/>
+      <c r="F29" s="62"/>
+      <c r="G29" s="49"/>
+      <c r="H29" s="64"/>
+      <c r="I29" s="62"/>
+      <c r="J29" s="49"/>
+      <c r="K29" s="54"/>
+      <c r="L29" s="55"/>
+      <c r="M29" s="55"/>
+      <c r="N29" s="55"/>
+      <c r="O29" s="55"/>
+      <c r="P29" s="55"/>
+      <c r="Q29" s="43"/>
       <c r="R29" s="1"/>
     </row>
-    <row r="30" ht="15.75" customHeight="1">
+    <row r="30" spans="1:18" ht="15.75" customHeight="1">
       <c r="A30" s="1"/>
-      <c r="B30" s="22"/>
-      <c r="C30" s="18"/>
-      <c r="D30" s="18"/>
-      <c r="E30" s="18"/>
-      <c r="F30" s="18"/>
-      <c r="G30" s="23"/>
-      <c r="H30" s="22"/>
-      <c r="I30" s="18"/>
-      <c r="J30" s="23"/>
-      <c r="K30" s="71" t="s">
-        <v>52</v>
-      </c>
-      <c r="L30" s="18"/>
-      <c r="M30" s="18"/>
-      <c r="N30" s="18"/>
-      <c r="O30" s="18"/>
-      <c r="P30" s="18"/>
-      <c r="Q30" s="23"/>
+      <c r="B30" s="54"/>
+      <c r="C30" s="55"/>
+      <c r="D30" s="55"/>
+      <c r="E30" s="55"/>
+      <c r="F30" s="55"/>
+      <c r="G30" s="43"/>
+      <c r="H30" s="54"/>
+      <c r="I30" s="55"/>
+      <c r="J30" s="43"/>
+      <c r="K30" s="69" t="s">
+        <v>51</v>
+      </c>
+      <c r="L30" s="55"/>
+      <c r="M30" s="55"/>
+      <c r="N30" s="55"/>
+      <c r="O30" s="55"/>
+      <c r="P30" s="55"/>
+      <c r="Q30" s="43"/>
       <c r="R30" s="1"/>
     </row>
-    <row r="31" ht="3.75" customHeight="1">
+    <row r="31" spans="1:18" ht="3.75" customHeight="1">
       <c r="A31" s="1"/>
-      <c r="B31" s="95"/>
-      <c r="C31" s="95"/>
-      <c r="D31" s="95"/>
-      <c r="E31" s="95"/>
-      <c r="F31" s="95"/>
-      <c r="G31" s="95"/>
-      <c r="H31" s="95"/>
-      <c r="I31" s="95"/>
-      <c r="J31" s="95"/>
-      <c r="K31" s="95"/>
-      <c r="L31" s="95"/>
-      <c r="M31" s="95"/>
-      <c r="N31" s="95"/>
-      <c r="O31" s="95"/>
-      <c r="P31" s="95"/>
-      <c r="Q31" s="95"/>
+      <c r="B31" s="18"/>
+      <c r="C31" s="18"/>
+      <c r="D31" s="18"/>
+      <c r="E31" s="18"/>
+      <c r="F31" s="18"/>
+      <c r="G31" s="18"/>
+      <c r="H31" s="18"/>
+      <c r="I31" s="18"/>
+      <c r="J31" s="18"/>
+      <c r="K31" s="18"/>
+      <c r="L31" s="18"/>
+      <c r="M31" s="18"/>
+      <c r="N31" s="18"/>
+      <c r="O31" s="18"/>
+      <c r="P31" s="18"/>
+      <c r="Q31" s="18"/>
       <c r="R31" s="1"/>
     </row>
-    <row r="32" ht="15.75" customHeight="1">
-      <c r="B32" s="64" t="s">
-        <v>53</v>
-      </c>
+    <row r="32" spans="1:18" ht="15.75" customHeight="1">
+      <c r="B32" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="C32" s="62"/>
+      <c r="D32" s="62"/>
+      <c r="E32" s="62"/>
+      <c r="F32" s="62"/>
+      <c r="G32" s="62"/>
+      <c r="H32" s="62"/>
+      <c r="I32" s="62"/>
+      <c r="J32" s="62"/>
+      <c r="K32" s="62"/>
+      <c r="L32" s="62"/>
+      <c r="M32" s="62"/>
+      <c r="N32" s="62"/>
+      <c r="O32" s="62"/>
+      <c r="P32" s="62"/>
+      <c r="Q32" s="62"/>
     </row>
     <row r="33" ht="15.75" customHeight="1"/>
     <row r="34" ht="15.75" customHeight="1"/>
@@ -2770,41 +3334,10 @@
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="55">
-    <mergeCell ref="K16:L17"/>
-    <mergeCell ref="K19:L19"/>
-    <mergeCell ref="K18:L18"/>
-    <mergeCell ref="B11:Q11"/>
-    <mergeCell ref="B12:Q12"/>
-    <mergeCell ref="I15:O15"/>
-    <mergeCell ref="B13:Q14"/>
-    <mergeCell ref="P16:Q17"/>
-    <mergeCell ref="M16:O16"/>
-    <mergeCell ref="N17:O17"/>
-    <mergeCell ref="N18:O18"/>
-    <mergeCell ref="P15:Q15"/>
-    <mergeCell ref="P18:Q18"/>
-    <mergeCell ref="B10:H10"/>
-    <mergeCell ref="B16:G17"/>
-    <mergeCell ref="B15:H15"/>
-    <mergeCell ref="J16:J17"/>
-    <mergeCell ref="B19:G19"/>
-    <mergeCell ref="J10:Q10"/>
-    <mergeCell ref="B18:G18"/>
-    <mergeCell ref="K26:Q29"/>
-    <mergeCell ref="K24:Q25"/>
-    <mergeCell ref="K30:Q30"/>
-    <mergeCell ref="B32:Q32"/>
-    <mergeCell ref="B27:G30"/>
-    <mergeCell ref="H23:J30"/>
-    <mergeCell ref="P23:Q23"/>
-    <mergeCell ref="K23:O23"/>
-    <mergeCell ref="B21:J22"/>
-    <mergeCell ref="B23:G23"/>
-    <mergeCell ref="B24:G24"/>
-    <mergeCell ref="K22:O22"/>
-    <mergeCell ref="P22:Q22"/>
-    <mergeCell ref="B26:G26"/>
-    <mergeCell ref="B25:G25"/>
+    <mergeCell ref="B2:Q2"/>
+    <mergeCell ref="B3:C4"/>
+    <mergeCell ref="P21:Q21"/>
+    <mergeCell ref="K21:O21"/>
     <mergeCell ref="F3:N3"/>
     <mergeCell ref="O3:Q4"/>
     <mergeCell ref="H16:H17"/>
@@ -2821,13 +3354,44 @@
     <mergeCell ref="B8:I8"/>
     <mergeCell ref="J8:Q8"/>
     <mergeCell ref="B6:Q7"/>
-    <mergeCell ref="B2:Q2"/>
-    <mergeCell ref="B3:C4"/>
-    <mergeCell ref="P21:Q21"/>
-    <mergeCell ref="K21:O21"/>
+    <mergeCell ref="B21:J22"/>
+    <mergeCell ref="B23:G23"/>
+    <mergeCell ref="B24:G24"/>
+    <mergeCell ref="K22:O22"/>
+    <mergeCell ref="P22:Q22"/>
+    <mergeCell ref="K26:Q29"/>
+    <mergeCell ref="K24:Q25"/>
+    <mergeCell ref="K30:Q30"/>
+    <mergeCell ref="B32:Q32"/>
+    <mergeCell ref="B27:G30"/>
+    <mergeCell ref="H23:J30"/>
+    <mergeCell ref="P23:Q23"/>
+    <mergeCell ref="K23:O23"/>
+    <mergeCell ref="B26:G26"/>
+    <mergeCell ref="B25:G25"/>
+    <mergeCell ref="B10:H10"/>
+    <mergeCell ref="B16:G17"/>
+    <mergeCell ref="B15:H15"/>
+    <mergeCell ref="J16:J17"/>
+    <mergeCell ref="B19:G19"/>
+    <mergeCell ref="J10:Q10"/>
+    <mergeCell ref="B18:G18"/>
+    <mergeCell ref="K16:L17"/>
+    <mergeCell ref="K19:L19"/>
+    <mergeCell ref="K18:L18"/>
+    <mergeCell ref="B11:Q11"/>
+    <mergeCell ref="B12:Q12"/>
+    <mergeCell ref="I15:O15"/>
+    <mergeCell ref="B13:Q14"/>
+    <mergeCell ref="P16:Q17"/>
+    <mergeCell ref="M16:O16"/>
+    <mergeCell ref="N17:O17"/>
+    <mergeCell ref="N18:O18"/>
+    <mergeCell ref="P15:Q15"/>
+    <mergeCell ref="P18:Q18"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.25" right="0.25" top="0.75"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
CRM-2862 Change 247around tax invoice template and excel format, delivery challan and jobcart make main partner detail dynamic.
</commit_message>
<xml_diff>
--- a/application/controllers/excel-templates/247around_Tax_Invoice_Inter_State.xlsx
+++ b/application/controllers/excel-templates/247around_Tax_Invoice_Inter_State.xlsx
@@ -1,31 +1,36 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\247around-adminp-aws\application\controllers\excel-templates\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AF75511-8663-48C9-8088-52E8E7DB9C06}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Tax Invoice - Inter State" sheetId="1" r:id="rId3"/>
+    <sheet name="Tax Invoice - Inter State" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="54">
   <si>
-    <t>Blackmelon Advance Technology Co. Pvt. Ltd.</t>
-  </si>
-  <si>
-    <t>A-1/7a, A BLOCK, KRISHNA NAGAR, DELHI 110051</t>
-  </si>
-  <si>
     <t>({meta:recipient_type})</t>
-  </si>
-  <si>
-    <t>Email: seller@247around.com</t>
-  </si>
-  <si>
-    <t>GSTIN: 07AAFCB1281J1ZQ</t>
   </si>
   <si>
     <t>{meta:invoice_type}</t>
@@ -158,83 +163,98 @@
     <t>GST on Reverse Charge</t>
   </si>
   <si>
-    <t>Bank Name: ICICI Bank</t>
-  </si>
-  <si>
-    <t>For Blackmelon Advance Technology Co. Pvt. Ltd.</t>
-  </si>
-  <si>
-    <t>Acc No: 102405500277</t>
-  </si>
-  <si>
-    <t>IFSC: ICIC0001024</t>
-  </si>
-  <si>
     <t>Authorised signatory</t>
   </si>
   <si>
     <t>This is a computer generated invoice, no signature is required.</t>
+  </si>
+  <si>
+    <t>{meta:main_company_name}</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> {meta:main_company_address}, {meta:main_company_state}, {meta:main_company_pincode}</t>
+  </si>
+  <si>
+    <t>Email: {meta:main_company_email}</t>
+  </si>
+  <si>
+    <t>GSTIN: {meta:main_company_gst_number}</t>
+  </si>
+  <si>
+    <t>For {meta:main_company_name}</t>
+  </si>
+  <si>
+    <t>Bank Name: {meta:main_company_bank_name}</t>
+  </si>
+  <si>
+    <t>Acc No: {meta:main_company_bank_account}</t>
+  </si>
+  <si>
+    <t>IFSC: {meta:main_company_ifsc_code}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="11">
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
       <b/>
-      <sz val="18.0"/>
+      <sz val="18"/>
       <color rgb="FF000000"/>
       <name val="Bookman Old Style"/>
     </font>
-    <font/>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
     <font>
       <b/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
       <b/>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Bookman Old Style"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Bookman Old Style"/>
     </font>
     <font>
       <b/>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Bookman Old Style"/>
     </font>
     <font>
-      <sz val="14.0"/>
+      <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
       <b/>
-      <sz val="14.0"/>
+      <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
       <b/>
-      <sz val="14.0"/>
+      <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="Bookman Old Style"/>
     </font>
@@ -244,7 +264,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -254,79 +274,119 @@
     </fill>
   </fills>
   <borders count="53">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left style="medium">
         <color rgb="FF000000"/>
       </left>
+      <right/>
       <top style="medium">
         <color rgb="FF000000"/>
       </top>
-    </border>
-    <border>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="medium">
         <color rgb="FF000000"/>
       </top>
-    </border>
-    <border>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="medium">
         <color rgb="FF000000"/>
       </right>
       <top style="medium">
         <color rgb="FF000000"/>
       </top>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="medium">
         <color rgb="FF000000"/>
       </left>
-    </border>
-    <border>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="medium">
         <color rgb="FF000000"/>
       </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="medium">
         <color rgb="FF000000"/>
       </left>
+      <right/>
+      <top/>
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
-    </border>
-    <border>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
-    </border>
-    <border>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="medium">
         <color rgb="FF000000"/>
       </right>
+      <top/>
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="medium">
         <color rgb="FF000000"/>
       </left>
+      <right/>
       <top style="medium">
         <color rgb="FF000000"/>
       </top>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
-    </border>
-    <border>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="medium">
         <color rgb="FF000000"/>
       </top>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
-    </border>
-    <border>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="medium">
         <color rgb="FF000000"/>
       </right>
@@ -336,27 +396,34 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="medium">
         <color rgb="FF000000"/>
       </left>
+      <right/>
       <top style="medium">
         <color rgb="FF000000"/>
       </top>
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
-    </border>
-    <border>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="medium">
         <color rgb="FF000000"/>
       </top>
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
-    </border>
-    <border>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="medium">
         <color rgb="FF000000"/>
       </right>
@@ -366,27 +433,34 @@
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="medium">
         <color rgb="FF000000"/>
       </left>
+      <right/>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
-    </border>
-    <border>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
-    </border>
-    <border>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="medium">
         <color rgb="FF000000"/>
       </right>
@@ -396,6 +470,7 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -410,72 +485,102 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="medium">
         <color rgb="FF000000"/>
       </left>
+      <right/>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
-    </border>
-    <border>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
-    </border>
-    <border>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="medium">
         <color rgb="FF000000"/>
       </right>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="medium">
         <color rgb="FF000000"/>
       </left>
+      <right/>
+      <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
-    </border>
-    <border>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
-    </border>
-    <border>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="medium">
         <color rgb="FF000000"/>
       </right>
+      <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
-    </border>
-    <border>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
+      <right/>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
-    </border>
-    <border>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
       <top style="medium">
         <color rgb="FF000000"/>
       </top>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -487,27 +592,35 @@
       <top style="medium">
         <color rgb="FF000000"/>
       </top>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
+      <right/>
       <top style="medium">
         <color rgb="FF000000"/>
       </top>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
+      <right/>
       <top style="medium">
         <color rgb="FF000000"/>
       </top>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
-    </border>
-    <border>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
@@ -517,14 +630,18 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
-    </border>
-    <border>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
+      <top/>
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -533,17 +650,22 @@
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
+      <top/>
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
+      <right/>
+      <top/>
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -558,19 +680,23 @@
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
+      <right/>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
-    </border>
-    <border>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
@@ -580,11 +706,16 @@
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
-    </border>
-    <border>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -593,8 +724,12 @@
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
-    </border>
-    <border>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
@@ -604,6 +739,7 @@
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -618,16 +754,21 @@
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
-    </border>
-    <border>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
+      <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
-    </border>
-    <border>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
@@ -637,27 +778,34 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="medium">
         <color rgb="FF000000"/>
       </left>
+      <right/>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
-    </border>
-    <border>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
-    </border>
-    <border>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="medium">
         <color rgb="FF000000"/>
       </right>
@@ -667,449 +815,628 @@
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="medium">
         <color rgb="FF000000"/>
       </left>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom/>
-    </border>
-    <border>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom/>
-    </border>
-    <border>
       <right/>
       <top style="medium">
         <color rgb="FF000000"/>
       </top>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="medium">
         <color rgb="FF000000"/>
       </left>
+      <right/>
+      <top/>
       <bottom/>
-    </border>
-    <border>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom/>
-    </border>
-    <border>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="medium">
         <color rgb="FF000000"/>
       </right>
+      <top/>
       <bottom/>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="96">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+  <cellXfs count="98">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="3" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="4" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="5" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="4" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="6" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="7" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="7" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf borderId="7" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="7" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="7" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf borderId="8" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="6" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="8" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="9" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf borderId="10" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="11" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="12" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf borderId="13" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="14" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="15" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf borderId="16" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="17" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="10" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf borderId="18" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="12" fillId="2" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="19" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="20" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="21" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="22" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="23" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="24" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="19" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf borderId="20" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="9" fillId="0" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf borderId="25" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="26" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="27" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="28" fillId="2" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="28" fillId="2" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="29" fillId="2" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="30" fillId="2" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="31" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="29" fillId="2" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="32" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="33" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="34" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="35" fillId="2" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="36" fillId="2" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="37" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="4" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="38" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="39" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="38" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="12" fillId="2" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="40" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="41" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf borderId="41" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="13" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="6" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="22" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf borderId="42" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="22" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="15" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf borderId="43" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="15" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="44" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf borderId="45" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="44" fillId="0" fontId="9" numFmtId="1" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="46" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="47" fillId="2" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="48" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="49" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="13" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf borderId="12" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="1" fillId="2" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="44" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf borderId="50" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="51" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="52" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram">
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>95250</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="533400" cy="619125"/>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image1.png" title="Image"/>
-        <xdr:cNvPicPr preferRelativeResize="0"/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip cstate="print" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData fLocksWithSheet="0"/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>276225</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="1133475" cy="1095375"/>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image2.jpg" title="Image"/>
-        <xdr:cNvPicPr preferRelativeResize="0"/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip cstate="print" r:embed="rId2"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData fLocksWithSheet="0"/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>142875</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="1190625" cy="342900"/>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image3.png" title="Image"/>
-        <xdr:cNvPicPr preferRelativeResize="0"/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip cstate="print" r:embed="rId3"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData fLocksWithSheet="0"/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>85725</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="523875" cy="628650"/>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image4.png"/>
-        <xdr:cNvPicPr preferRelativeResize="0"/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip cstate="print" r:embed="rId4"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData fLocksWithSheet="0"/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>85725</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="523875" cy="628650"/>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image4.png"/>
-        <xdr:cNvPicPr preferRelativeResize="0"/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip cstate="print" r:embed="rId4"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData fLocksWithSheet="0"/>
-  </xdr:oneCellAnchor>
-</xdr:wsDr>
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:R1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="T20" sqref="T20"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="0.86"/>
-    <col customWidth="1" min="2" max="2" width="2.71"/>
-    <col customWidth="1" min="3" max="3" width="7.29"/>
-    <col customWidth="1" min="4" max="4" width="4.14"/>
-    <col customWidth="1" min="5" max="5" width="5.29"/>
-    <col customWidth="1" min="6" max="6" width="3.71"/>
-    <col customWidth="1" min="7" max="7" width="6.14"/>
-    <col customWidth="1" min="8" max="8" width="9.71"/>
-    <col customWidth="1" min="9" max="9" width="6.14"/>
-    <col customWidth="1" min="10" max="10" width="10.0"/>
-    <col customWidth="1" min="11" max="11" width="1.14"/>
-    <col customWidth="1" min="12" max="12" width="9.86"/>
-    <col customWidth="1" min="13" max="13" width="5.14"/>
-    <col customWidth="1" min="14" max="14" width="4.29"/>
-    <col customWidth="1" min="15" max="15" width="6.14"/>
-    <col customWidth="1" min="16" max="16" width="5.43"/>
-    <col customWidth="1" min="17" max="17" width="8.71"/>
-    <col customWidth="1" min="18" max="18" width="0.86"/>
+    <col min="1" max="1" width="0.88671875" customWidth="1"/>
+    <col min="2" max="2" width="2.6640625" customWidth="1"/>
+    <col min="3" max="3" width="7.33203125" customWidth="1"/>
+    <col min="4" max="4" width="4.109375" customWidth="1"/>
+    <col min="5" max="5" width="5.33203125" customWidth="1"/>
+    <col min="6" max="6" width="3.6640625" customWidth="1"/>
+    <col min="7" max="7" width="6.109375" customWidth="1"/>
+    <col min="8" max="8" width="9.6640625" customWidth="1"/>
+    <col min="9" max="9" width="6.109375" customWidth="1"/>
+    <col min="10" max="10" width="10" customWidth="1"/>
+    <col min="11" max="11" width="1.109375" customWidth="1"/>
+    <col min="12" max="12" width="9.88671875" customWidth="1"/>
+    <col min="13" max="13" width="5.109375" customWidth="1"/>
+    <col min="14" max="14" width="4.33203125" customWidth="1"/>
+    <col min="15" max="15" width="6.109375" customWidth="1"/>
+    <col min="16" max="16" width="5.44140625" customWidth="1"/>
+    <col min="17" max="17" width="8.6640625" customWidth="1"/>
+    <col min="18" max="18" width="0.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="3.75" customHeight="1">
+    <row r="1" spans="1:18" ht="3.75" customHeight="1">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -1129,676 +1456,738 @@
       <c r="Q1" s="1"/>
       <c r="R1" s="1"/>
     </row>
-    <row r="2" ht="29.25" customHeight="1">
+    <row r="2" spans="1:18" ht="29.25" customHeight="1">
       <c r="A2" s="1"/>
-      <c r="B2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
-      <c r="M2" s="3"/>
-      <c r="N2" s="3"/>
-      <c r="O2" s="3"/>
-      <c r="P2" s="3"/>
-      <c r="Q2" s="4"/>
+      <c r="B2" s="50" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" s="51"/>
+      <c r="D2" s="51"/>
+      <c r="E2" s="51"/>
+      <c r="F2" s="51"/>
+      <c r="G2" s="51"/>
+      <c r="H2" s="51"/>
+      <c r="I2" s="51"/>
+      <c r="J2" s="51"/>
+      <c r="K2" s="51"/>
+      <c r="L2" s="51"/>
+      <c r="M2" s="51"/>
+      <c r="N2" s="51"/>
+      <c r="O2" s="51"/>
+      <c r="P2" s="51"/>
+      <c r="Q2" s="52"/>
       <c r="R2" s="1"/>
     </row>
-    <row r="3" ht="30.0" customHeight="1">
+    <row r="3" spans="1:18" ht="30" customHeight="1">
       <c r="A3" s="1"/>
-      <c r="B3" s="5"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="O3" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q3" s="9"/>
+      <c r="B3" s="53"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="G3" s="25"/>
+      <c r="H3" s="25"/>
+      <c r="I3" s="25"/>
+      <c r="J3" s="25"/>
+      <c r="K3" s="25"/>
+      <c r="L3" s="25"/>
+      <c r="M3" s="25"/>
+      <c r="N3" s="25"/>
+      <c r="O3" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="P3" s="25"/>
+      <c r="Q3" s="27"/>
       <c r="R3" s="1"/>
     </row>
-    <row r="4">
+    <row r="4" spans="1:18" ht="15.6">
       <c r="A4" s="1"/>
-      <c r="B4" s="10"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="N4" s="13"/>
-      <c r="Q4" s="9"/>
+      <c r="B4" s="54"/>
+      <c r="C4" s="25"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="67" t="s">
+        <v>48</v>
+      </c>
+      <c r="H4" s="25"/>
+      <c r="I4" s="25"/>
+      <c r="J4" s="25"/>
+      <c r="K4" s="25"/>
+      <c r="L4" s="25"/>
+      <c r="M4" s="25"/>
+      <c r="N4" s="5"/>
+      <c r="O4" s="25"/>
+      <c r="P4" s="25"/>
+      <c r="Q4" s="27"/>
       <c r="R4" s="1"/>
     </row>
-    <row r="5">
+    <row r="5" spans="1:18" ht="15.6">
       <c r="A5" s="1"/>
-      <c r="B5" s="14"/>
-      <c r="C5" s="15"/>
-      <c r="D5" s="16"/>
-      <c r="E5" s="16"/>
-      <c r="F5" s="16"/>
-      <c r="G5" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="H5" s="18"/>
-      <c r="I5" s="18"/>
-      <c r="J5" s="18"/>
-      <c r="K5" s="18"/>
-      <c r="L5" s="18"/>
-      <c r="M5" s="18"/>
-      <c r="N5" s="17"/>
-      <c r="O5" s="17"/>
-      <c r="P5" s="19"/>
-      <c r="Q5" s="20"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="45" t="s">
+        <v>49</v>
+      </c>
+      <c r="H5" s="32"/>
+      <c r="I5" s="32"/>
+      <c r="J5" s="32"/>
+      <c r="K5" s="32"/>
+      <c r="L5" s="32"/>
+      <c r="M5" s="32"/>
+      <c r="N5" s="9"/>
+      <c r="O5" s="9"/>
+      <c r="P5" s="10"/>
+      <c r="Q5" s="11"/>
       <c r="R5" s="1"/>
     </row>
-    <row r="6" ht="15.75" customHeight="1">
+    <row r="6" spans="1:18" ht="15.75" customHeight="1">
       <c r="A6" s="1"/>
-      <c r="B6" s="21" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
-      <c r="L6" s="3"/>
-      <c r="M6" s="3"/>
-      <c r="N6" s="3"/>
-      <c r="O6" s="3"/>
-      <c r="P6" s="3"/>
-      <c r="Q6" s="4"/>
+      <c r="B6" s="70" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="51"/>
+      <c r="D6" s="51"/>
+      <c r="E6" s="51"/>
+      <c r="F6" s="51"/>
+      <c r="G6" s="51"/>
+      <c r="H6" s="51"/>
+      <c r="I6" s="51"/>
+      <c r="J6" s="51"/>
+      <c r="K6" s="51"/>
+      <c r="L6" s="51"/>
+      <c r="M6" s="51"/>
+      <c r="N6" s="51"/>
+      <c r="O6" s="51"/>
+      <c r="P6" s="51"/>
+      <c r="Q6" s="52"/>
       <c r="R6" s="1"/>
     </row>
-    <row r="7" ht="7.5" customHeight="1">
+    <row r="7" spans="1:18" ht="7.5" customHeight="1">
       <c r="A7" s="1"/>
-      <c r="B7" s="22"/>
-      <c r="C7" s="18"/>
-      <c r="D7" s="18"/>
-      <c r="E7" s="18"/>
-      <c r="F7" s="18"/>
-      <c r="G7" s="18"/>
-      <c r="H7" s="18"/>
-      <c r="I7" s="18"/>
-      <c r="J7" s="18"/>
-      <c r="K7" s="18"/>
-      <c r="L7" s="18"/>
-      <c r="M7" s="18"/>
-      <c r="N7" s="18"/>
-      <c r="O7" s="18"/>
-      <c r="P7" s="18"/>
-      <c r="Q7" s="23"/>
+      <c r="B7" s="61"/>
+      <c r="C7" s="32"/>
+      <c r="D7" s="32"/>
+      <c r="E7" s="32"/>
+      <c r="F7" s="32"/>
+      <c r="G7" s="32"/>
+      <c r="H7" s="32"/>
+      <c r="I7" s="32"/>
+      <c r="J7" s="32"/>
+      <c r="K7" s="32"/>
+      <c r="L7" s="32"/>
+      <c r="M7" s="32"/>
+      <c r="N7" s="32"/>
+      <c r="O7" s="32"/>
+      <c r="P7" s="32"/>
+      <c r="Q7" s="62"/>
       <c r="R7" s="1"/>
     </row>
-    <row r="8" ht="21.75" customHeight="1">
+    <row r="8" spans="1:18" ht="21.75" customHeight="1">
       <c r="A8" s="1"/>
-      <c r="B8" s="24" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" s="25"/>
-      <c r="D8" s="25"/>
-      <c r="E8" s="25"/>
-      <c r="F8" s="25"/>
-      <c r="G8" s="25"/>
-      <c r="H8" s="25"/>
-      <c r="I8" s="26"/>
-      <c r="J8" s="27" t="s">
-        <v>7</v>
-      </c>
-      <c r="K8" s="28"/>
-      <c r="L8" s="28"/>
-      <c r="M8" s="28"/>
-      <c r="N8" s="28"/>
-      <c r="O8" s="28"/>
-      <c r="P8" s="28"/>
-      <c r="Q8" s="29"/>
+      <c r="B8" s="68" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" s="43"/>
+      <c r="D8" s="43"/>
+      <c r="E8" s="43"/>
+      <c r="F8" s="43"/>
+      <c r="G8" s="43"/>
+      <c r="H8" s="43"/>
+      <c r="I8" s="44"/>
+      <c r="J8" s="69" t="s">
+        <v>3</v>
+      </c>
+      <c r="K8" s="49"/>
+      <c r="L8" s="49"/>
+      <c r="M8" s="49"/>
+      <c r="N8" s="49"/>
+      <c r="O8" s="49"/>
+      <c r="P8" s="49"/>
+      <c r="Q8" s="39"/>
       <c r="R8" s="1"/>
     </row>
-    <row r="9" ht="21.0" customHeight="1">
+    <row r="9" spans="1:18" ht="21" customHeight="1">
       <c r="A9" s="1"/>
-      <c r="B9" s="30" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" s="31"/>
-      <c r="D9" s="31"/>
-      <c r="E9" s="31"/>
-      <c r="F9" s="31"/>
-      <c r="G9" s="31"/>
-      <c r="H9" s="31"/>
-      <c r="I9" s="32"/>
-      <c r="J9" s="33" t="s">
-        <v>9</v>
-      </c>
-      <c r="K9" s="25"/>
-      <c r="L9" s="25"/>
-      <c r="M9" s="25"/>
-      <c r="N9" s="25"/>
-      <c r="O9" s="25"/>
-      <c r="P9" s="25"/>
-      <c r="Q9" s="26"/>
+      <c r="B9" s="41" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="22"/>
+      <c r="D9" s="22"/>
+      <c r="E9" s="22"/>
+      <c r="F9" s="22"/>
+      <c r="G9" s="22"/>
+      <c r="H9" s="22"/>
+      <c r="I9" s="20"/>
+      <c r="J9" s="42" t="s">
+        <v>5</v>
+      </c>
+      <c r="K9" s="43"/>
+      <c r="L9" s="43"/>
+      <c r="M9" s="43"/>
+      <c r="N9" s="43"/>
+      <c r="O9" s="43"/>
+      <c r="P9" s="43"/>
+      <c r="Q9" s="44"/>
       <c r="R9" s="1"/>
     </row>
-    <row r="10" ht="19.5" customHeight="1">
+    <row r="10" spans="1:18" ht="19.5" customHeight="1">
       <c r="A10" s="1"/>
-      <c r="B10" s="30" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" s="31"/>
-      <c r="D10" s="31"/>
-      <c r="E10" s="31"/>
-      <c r="F10" s="31"/>
-      <c r="G10" s="31"/>
-      <c r="H10" s="31"/>
-      <c r="I10" s="34" t="s">
-        <v>11</v>
-      </c>
-      <c r="J10" s="33"/>
-      <c r="K10" s="25"/>
-      <c r="L10" s="25"/>
-      <c r="M10" s="25"/>
-      <c r="N10" s="25"/>
-      <c r="O10" s="25"/>
-      <c r="P10" s="25"/>
-      <c r="Q10" s="26"/>
+      <c r="B10" s="41" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="22"/>
+      <c r="D10" s="22"/>
+      <c r="E10" s="22"/>
+      <c r="F10" s="22"/>
+      <c r="G10" s="22"/>
+      <c r="H10" s="22"/>
+      <c r="I10" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="J10" s="42"/>
+      <c r="K10" s="43"/>
+      <c r="L10" s="43"/>
+      <c r="M10" s="43"/>
+      <c r="N10" s="43"/>
+      <c r="O10" s="43"/>
+      <c r="P10" s="43"/>
+      <c r="Q10" s="44"/>
       <c r="R10" s="1"/>
     </row>
-    <row r="11">
+    <row r="11" spans="1:18" ht="18">
       <c r="A11" s="1"/>
-      <c r="B11" s="35" t="s">
-        <v>12</v>
-      </c>
-      <c r="C11" s="28"/>
-      <c r="D11" s="28"/>
-      <c r="E11" s="28"/>
-      <c r="F11" s="28"/>
-      <c r="G11" s="28"/>
-      <c r="H11" s="28"/>
-      <c r="I11" s="28"/>
-      <c r="J11" s="28"/>
-      <c r="K11" s="28"/>
-      <c r="L11" s="28"/>
-      <c r="M11" s="28"/>
-      <c r="N11" s="28"/>
-      <c r="O11" s="28"/>
-      <c r="P11" s="28"/>
-      <c r="Q11" s="29"/>
+      <c r="B11" s="48" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="49"/>
+      <c r="D11" s="49"/>
+      <c r="E11" s="49"/>
+      <c r="F11" s="49"/>
+      <c r="G11" s="49"/>
+      <c r="H11" s="49"/>
+      <c r="I11" s="49"/>
+      <c r="J11" s="49"/>
+      <c r="K11" s="49"/>
+      <c r="L11" s="49"/>
+      <c r="M11" s="49"/>
+      <c r="N11" s="49"/>
+      <c r="O11" s="49"/>
+      <c r="P11" s="49"/>
+      <c r="Q11" s="39"/>
       <c r="R11" s="1"/>
     </row>
-    <row r="12" ht="24.75" customHeight="1">
+    <row r="12" spans="1:18" ht="24.75" customHeight="1">
       <c r="A12" s="1"/>
-      <c r="B12" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="C12" s="25"/>
-      <c r="D12" s="25"/>
-      <c r="E12" s="25"/>
-      <c r="F12" s="25"/>
-      <c r="G12" s="25"/>
-      <c r="H12" s="25"/>
-      <c r="I12" s="25"/>
-      <c r="J12" s="25"/>
-      <c r="K12" s="25"/>
-      <c r="L12" s="25"/>
-      <c r="M12" s="25"/>
-      <c r="N12" s="25"/>
-      <c r="O12" s="25"/>
-      <c r="P12" s="25"/>
-      <c r="Q12" s="26"/>
+      <c r="B12" s="68" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="43"/>
+      <c r="D12" s="43"/>
+      <c r="E12" s="43"/>
+      <c r="F12" s="43"/>
+      <c r="G12" s="43"/>
+      <c r="H12" s="43"/>
+      <c r="I12" s="43"/>
+      <c r="J12" s="43"/>
+      <c r="K12" s="43"/>
+      <c r="L12" s="43"/>
+      <c r="M12" s="43"/>
+      <c r="N12" s="43"/>
+      <c r="O12" s="43"/>
+      <c r="P12" s="43"/>
+      <c r="Q12" s="44"/>
       <c r="R12" s="1"/>
     </row>
-    <row r="13">
+    <row r="13" spans="1:18" ht="14.4">
       <c r="A13" s="1"/>
-      <c r="B13" s="36" t="s">
-        <v>14</v>
-      </c>
-      <c r="C13" s="37"/>
-      <c r="D13" s="37"/>
-      <c r="E13" s="37"/>
-      <c r="F13" s="37"/>
-      <c r="G13" s="37"/>
-      <c r="H13" s="37"/>
-      <c r="I13" s="37"/>
-      <c r="J13" s="37"/>
-      <c r="K13" s="37"/>
-      <c r="L13" s="37"/>
-      <c r="M13" s="37"/>
-      <c r="N13" s="37"/>
-      <c r="O13" s="37"/>
-      <c r="P13" s="37"/>
-      <c r="Q13" s="38"/>
+      <c r="B13" s="91" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" s="76"/>
+      <c r="D13" s="76"/>
+      <c r="E13" s="76"/>
+      <c r="F13" s="76"/>
+      <c r="G13" s="76"/>
+      <c r="H13" s="76"/>
+      <c r="I13" s="76"/>
+      <c r="J13" s="76"/>
+      <c r="K13" s="76"/>
+      <c r="L13" s="76"/>
+      <c r="M13" s="76"/>
+      <c r="N13" s="76"/>
+      <c r="O13" s="76"/>
+      <c r="P13" s="76"/>
+      <c r="Q13" s="88"/>
       <c r="R13" s="1"/>
     </row>
-    <row r="14" ht="15.75" customHeight="1">
+    <row r="14" spans="1:18" ht="15.75" customHeight="1">
       <c r="A14" s="1"/>
-      <c r="B14" s="39"/>
-      <c r="C14" s="40"/>
-      <c r="D14" s="40"/>
-      <c r="E14" s="40"/>
-      <c r="F14" s="40"/>
-      <c r="G14" s="40"/>
-      <c r="H14" s="40"/>
-      <c r="I14" s="40"/>
-      <c r="J14" s="40"/>
-      <c r="K14" s="40"/>
-      <c r="L14" s="40"/>
-      <c r="M14" s="40"/>
-      <c r="N14" s="40"/>
-      <c r="O14" s="40"/>
-      <c r="P14" s="40"/>
-      <c r="Q14" s="41"/>
+      <c r="B14" s="92"/>
+      <c r="C14" s="34"/>
+      <c r="D14" s="34"/>
+      <c r="E14" s="34"/>
+      <c r="F14" s="34"/>
+      <c r="G14" s="34"/>
+      <c r="H14" s="34"/>
+      <c r="I14" s="34"/>
+      <c r="J14" s="34"/>
+      <c r="K14" s="34"/>
+      <c r="L14" s="34"/>
+      <c r="M14" s="34"/>
+      <c r="N14" s="34"/>
+      <c r="O14" s="34"/>
+      <c r="P14" s="34"/>
+      <c r="Q14" s="37"/>
       <c r="R14" s="1"/>
     </row>
-    <row r="15" ht="25.5" customHeight="1">
+    <row r="15" spans="1:18" ht="25.5" customHeight="1">
       <c r="A15" s="1"/>
-      <c r="B15" s="42" t="s">
-        <v>15</v>
-      </c>
-      <c r="C15" s="37"/>
-      <c r="D15" s="37"/>
-      <c r="E15" s="37"/>
-      <c r="F15" s="37"/>
-      <c r="G15" s="37"/>
-      <c r="H15" s="37"/>
-      <c r="I15" s="43" t="s">
-        <v>16</v>
-      </c>
-      <c r="J15" s="37"/>
-      <c r="K15" s="37"/>
-      <c r="L15" s="37"/>
-      <c r="M15" s="37"/>
-      <c r="N15" s="37"/>
-      <c r="O15" s="44"/>
-      <c r="P15" s="45" t="s">
-        <v>17</v>
-      </c>
-      <c r="Q15" s="38"/>
+      <c r="B15" s="75" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" s="76"/>
+      <c r="D15" s="76"/>
+      <c r="E15" s="76"/>
+      <c r="F15" s="76"/>
+      <c r="G15" s="76"/>
+      <c r="H15" s="76"/>
+      <c r="I15" s="89" t="s">
+        <v>12</v>
+      </c>
+      <c r="J15" s="76"/>
+      <c r="K15" s="76"/>
+      <c r="L15" s="76"/>
+      <c r="M15" s="76"/>
+      <c r="N15" s="76"/>
+      <c r="O15" s="90"/>
+      <c r="P15" s="87" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q15" s="88"/>
       <c r="R15" s="1"/>
     </row>
-    <row r="16">
+    <row r="16" spans="1:18" ht="18">
       <c r="A16" s="1"/>
-      <c r="B16" s="46" t="s">
+      <c r="B16" s="72" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" s="51"/>
+      <c r="D16" s="51"/>
+      <c r="E16" s="51"/>
+      <c r="F16" s="51"/>
+      <c r="G16" s="73"/>
+      <c r="H16" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="I16" s="30" t="s">
+        <v>16</v>
+      </c>
+      <c r="J16" s="30" t="s">
+        <v>17</v>
+      </c>
+      <c r="K16" s="97" t="s">
         <v>18</v>
       </c>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="47"/>
-      <c r="H16" s="48" t="s">
+      <c r="L16" s="73"/>
+      <c r="M16" s="95" t="s">
         <v>19</v>
       </c>
-      <c r="I16" s="49" t="s">
+      <c r="N16" s="43"/>
+      <c r="O16" s="86"/>
+      <c r="P16" s="93" t="s">
         <v>20</v>
       </c>
-      <c r="J16" s="49" t="s">
-        <v>21</v>
-      </c>
-      <c r="K16" s="50" t="s">
-        <v>22</v>
-      </c>
-      <c r="L16" s="47"/>
-      <c r="M16" s="51" t="s">
-        <v>23</v>
-      </c>
-      <c r="N16" s="25"/>
-      <c r="O16" s="52"/>
-      <c r="P16" s="53" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q16" s="4"/>
+      <c r="Q16" s="52"/>
       <c r="R16" s="1"/>
     </row>
-    <row r="17" ht="25.5" customHeight="1">
+    <row r="17" spans="1:18" ht="25.5" customHeight="1">
       <c r="A17" s="1"/>
-      <c r="B17" s="22"/>
-      <c r="C17" s="18"/>
-      <c r="D17" s="18"/>
-      <c r="E17" s="18"/>
-      <c r="F17" s="18"/>
-      <c r="G17" s="54"/>
-      <c r="H17" s="55"/>
-      <c r="I17" s="55"/>
-      <c r="J17" s="55"/>
-      <c r="K17" s="56"/>
-      <c r="L17" s="54"/>
-      <c r="M17" s="57" t="s">
+      <c r="B17" s="61"/>
+      <c r="C17" s="32"/>
+      <c r="D17" s="32"/>
+      <c r="E17" s="32"/>
+      <c r="F17" s="32"/>
+      <c r="G17" s="74"/>
+      <c r="H17" s="29"/>
+      <c r="I17" s="29"/>
+      <c r="J17" s="29"/>
+      <c r="K17" s="94"/>
+      <c r="L17" s="74"/>
+      <c r="M17" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="N17" s="96" t="s">
         <v>21</v>
       </c>
-      <c r="N17" s="58" t="s">
-        <v>25</v>
-      </c>
-      <c r="O17" s="59"/>
-      <c r="P17" s="56"/>
-      <c r="Q17" s="23"/>
+      <c r="O17" s="57"/>
+      <c r="P17" s="94"/>
+      <c r="Q17" s="62"/>
       <c r="R17" s="1"/>
     </row>
-    <row r="18" ht="49.5" customHeight="1">
+    <row r="18" spans="1:18" ht="49.5" customHeight="1">
       <c r="A18" s="1"/>
-      <c r="B18" s="60" t="s">
+      <c r="B18" s="78" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" s="25"/>
+      <c r="D18" s="25"/>
+      <c r="E18" s="25"/>
+      <c r="F18" s="25"/>
+      <c r="G18" s="47"/>
+      <c r="H18" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="I18" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="J18" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="K18" s="46" t="s">
         <v>26</v>
       </c>
-      <c r="G18" s="61"/>
-      <c r="H18" s="62" t="s">
+      <c r="L18" s="47"/>
+      <c r="M18" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="I18" s="63" t="s">
+      <c r="N18" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="J18" s="62" t="s">
+      <c r="O18" s="47"/>
+      <c r="P18" s="46" t="s">
         <v>29</v>
       </c>
-      <c r="K18" s="64" t="s">
-        <v>30</v>
-      </c>
-      <c r="L18" s="61"/>
-      <c r="M18" s="62" t="s">
-        <v>31</v>
-      </c>
-      <c r="N18" s="64" t="s">
-        <v>32</v>
-      </c>
-      <c r="O18" s="61"/>
-      <c r="P18" s="65" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q18" s="9"/>
+      <c r="Q18" s="27"/>
       <c r="R18" s="1"/>
     </row>
-    <row r="19" ht="25.5" customHeight="1">
+    <row r="19" spans="1:18" ht="25.5" customHeight="1">
       <c r="A19" s="1"/>
-      <c r="B19" s="66" t="s">
-        <v>24</v>
-      </c>
-      <c r="C19" s="28"/>
-      <c r="D19" s="28"/>
-      <c r="E19" s="28"/>
-      <c r="F19" s="28"/>
-      <c r="G19" s="67"/>
-      <c r="H19" s="68"/>
-      <c r="I19" s="69" t="s">
-        <v>34</v>
-      </c>
-      <c r="J19" s="69"/>
-      <c r="K19" s="70" t="s">
-        <v>35</v>
-      </c>
-      <c r="L19" s="67"/>
-      <c r="M19" s="69"/>
-      <c r="N19" s="70" t="s">
-        <v>36</v>
-      </c>
-      <c r="O19" s="67"/>
-      <c r="P19" s="70" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q19" s="29"/>
+      <c r="B19" s="77" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19" s="49"/>
+      <c r="D19" s="49"/>
+      <c r="E19" s="49"/>
+      <c r="F19" s="49"/>
+      <c r="G19" s="40"/>
+      <c r="H19" s="16"/>
+      <c r="I19" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="J19" s="17"/>
+      <c r="K19" s="38" t="s">
+        <v>31</v>
+      </c>
+      <c r="L19" s="40"/>
+      <c r="M19" s="17"/>
+      <c r="N19" s="38" t="s">
+        <v>32</v>
+      </c>
+      <c r="O19" s="40"/>
+      <c r="P19" s="38" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q19" s="39"/>
       <c r="R19" s="1"/>
     </row>
-    <row r="20" ht="21.75" customHeight="1">
+    <row r="20" spans="1:18" ht="21.75" customHeight="1">
       <c r="A20" s="1"/>
-      <c r="B20" s="71" t="s">
-        <v>38</v>
-      </c>
-      <c r="C20" s="18"/>
-      <c r="D20" s="18"/>
-      <c r="E20" s="18"/>
-      <c r="F20" s="18"/>
-      <c r="G20" s="18"/>
-      <c r="H20" s="18"/>
-      <c r="I20" s="18"/>
-      <c r="J20" s="18"/>
-      <c r="K20" s="72" t="s">
-        <v>39</v>
-      </c>
-      <c r="L20" s="40"/>
-      <c r="M20" s="40"/>
-      <c r="N20" s="40"/>
-      <c r="O20" s="73"/>
-      <c r="P20" s="74" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q20" s="41"/>
+      <c r="B20" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="C20" s="32"/>
+      <c r="D20" s="32"/>
+      <c r="E20" s="32"/>
+      <c r="F20" s="32"/>
+      <c r="G20" s="32"/>
+      <c r="H20" s="32"/>
+      <c r="I20" s="32"/>
+      <c r="J20" s="32"/>
+      <c r="K20" s="33" t="s">
+        <v>35</v>
+      </c>
+      <c r="L20" s="34"/>
+      <c r="M20" s="34"/>
+      <c r="N20" s="34"/>
+      <c r="O20" s="35"/>
+      <c r="P20" s="36" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q20" s="37"/>
       <c r="R20" s="1"/>
     </row>
-    <row r="21" ht="15.75" customHeight="1">
+    <row r="21" spans="1:18" ht="15.75" customHeight="1">
       <c r="A21" s="1"/>
-      <c r="B21" s="75" t="s">
-        <v>41</v>
-      </c>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
-      <c r="H21" s="3"/>
-      <c r="I21" s="3"/>
-      <c r="J21" s="4"/>
-      <c r="K21" s="76" t="s">
-        <v>42</v>
-      </c>
-      <c r="L21" s="31"/>
-      <c r="M21" s="31"/>
-      <c r="N21" s="31"/>
-      <c r="O21" s="77"/>
-      <c r="P21" s="78" t="s">
-        <v>43</v>
-      </c>
-      <c r="Q21" s="32"/>
+      <c r="B21" s="71" t="s">
+        <v>37</v>
+      </c>
+      <c r="C21" s="51"/>
+      <c r="D21" s="51"/>
+      <c r="E21" s="51"/>
+      <c r="F21" s="51"/>
+      <c r="G21" s="51"/>
+      <c r="H21" s="51"/>
+      <c r="I21" s="51"/>
+      <c r="J21" s="52"/>
+      <c r="K21" s="21" t="s">
+        <v>38</v>
+      </c>
+      <c r="L21" s="22"/>
+      <c r="M21" s="22"/>
+      <c r="N21" s="22"/>
+      <c r="O21" s="23"/>
+      <c r="P21" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q21" s="20"/>
       <c r="R21" s="1"/>
     </row>
-    <row r="22" ht="24.0" customHeight="1">
+    <row r="22" spans="1:18" ht="24" customHeight="1">
       <c r="A22" s="1"/>
-      <c r="B22" s="22"/>
-      <c r="C22" s="18"/>
-      <c r="D22" s="18"/>
-      <c r="E22" s="18"/>
-      <c r="F22" s="18"/>
-      <c r="G22" s="18"/>
-      <c r="H22" s="18"/>
-      <c r="I22" s="18"/>
-      <c r="J22" s="23"/>
-      <c r="K22" s="79" t="s">
-        <v>44</v>
-      </c>
-      <c r="L22" s="80"/>
-      <c r="M22" s="80"/>
-      <c r="N22" s="80"/>
-      <c r="O22" s="59"/>
-      <c r="P22" s="81" t="s">
-        <v>45</v>
-      </c>
-      <c r="Q22" s="82"/>
+      <c r="B22" s="61"/>
+      <c r="C22" s="32"/>
+      <c r="D22" s="32"/>
+      <c r="E22" s="32"/>
+      <c r="F22" s="32"/>
+      <c r="G22" s="32"/>
+      <c r="H22" s="32"/>
+      <c r="I22" s="32"/>
+      <c r="J22" s="62"/>
+      <c r="K22" s="55" t="s">
+        <v>40</v>
+      </c>
+      <c r="L22" s="56"/>
+      <c r="M22" s="56"/>
+      <c r="N22" s="56"/>
+      <c r="O22" s="57"/>
+      <c r="P22" s="58" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q22" s="59"/>
       <c r="R22" s="1"/>
     </row>
-    <row r="23" ht="15.75" customHeight="1">
+    <row r="23" spans="1:18" ht="15.75" customHeight="1">
       <c r="A23" s="1"/>
       <c r="B23" s="83" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C23" s="84"/>
       <c r="D23" s="84"/>
       <c r="E23" s="84"/>
       <c r="F23" s="84"/>
       <c r="G23" s="85"/>
-      <c r="H23" s="86"/>
-      <c r="I23" s="3"/>
-      <c r="J23" s="4"/>
-      <c r="K23" s="87" t="s">
-        <v>47</v>
-      </c>
-      <c r="L23" s="28"/>
-      <c r="M23" s="28"/>
-      <c r="N23" s="28"/>
-      <c r="O23" s="29"/>
-      <c r="P23" s="88">
+      <c r="H23" s="60"/>
+      <c r="I23" s="51"/>
+      <c r="J23" s="52"/>
+      <c r="K23" s="81" t="s">
+        <v>43</v>
+      </c>
+      <c r="L23" s="49"/>
+      <c r="M23" s="49"/>
+      <c r="N23" s="49"/>
+      <c r="O23" s="39"/>
+      <c r="P23" s="80">
         <f>IF(I10="Y",P21,0)</f>
         <v>0</v>
       </c>
-      <c r="Q23" s="29"/>
+      <c r="Q23" s="39"/>
       <c r="R23" s="1"/>
     </row>
-    <row r="24" ht="15.75" customHeight="1">
+    <row r="24" spans="1:18" ht="15.75" customHeight="1">
       <c r="A24" s="1"/>
-      <c r="B24" s="24" t="s">
-        <v>48</v>
-      </c>
-      <c r="C24" s="25"/>
-      <c r="D24" s="25"/>
-      <c r="E24" s="25"/>
-      <c r="F24" s="25"/>
-      <c r="G24" s="52"/>
-      <c r="H24" s="10"/>
-      <c r="J24" s="9"/>
-      <c r="K24" s="89" t="s">
-        <v>49</v>
-      </c>
-      <c r="L24" s="3"/>
-      <c r="M24" s="3"/>
-      <c r="N24" s="3"/>
-      <c r="O24" s="3"/>
-      <c r="P24" s="3"/>
-      <c r="Q24" s="4"/>
+      <c r="B24" s="68" t="s">
+        <v>51</v>
+      </c>
+      <c r="C24" s="43"/>
+      <c r="D24" s="43"/>
+      <c r="E24" s="43"/>
+      <c r="F24" s="43"/>
+      <c r="G24" s="86"/>
+      <c r="H24" s="54"/>
+      <c r="I24" s="25"/>
+      <c r="J24" s="27"/>
+      <c r="K24" s="63" t="s">
+        <v>50</v>
+      </c>
+      <c r="L24" s="51"/>
+      <c r="M24" s="51"/>
+      <c r="N24" s="51"/>
+      <c r="O24" s="51"/>
+      <c r="P24" s="51"/>
+      <c r="Q24" s="52"/>
       <c r="R24" s="1"/>
     </row>
-    <row r="25" ht="15.75" customHeight="1">
+    <row r="25" spans="1:18" ht="15.75" customHeight="1">
       <c r="A25" s="1"/>
-      <c r="B25" s="90" t="s">
-        <v>50</v>
-      </c>
-      <c r="C25" s="80"/>
-      <c r="D25" s="80"/>
-      <c r="E25" s="80"/>
-      <c r="F25" s="80"/>
-      <c r="G25" s="59"/>
-      <c r="H25" s="10"/>
-      <c r="J25" s="9"/>
-      <c r="K25" s="91"/>
-      <c r="L25" s="92"/>
-      <c r="M25" s="92"/>
-      <c r="N25" s="92"/>
-      <c r="O25" s="92"/>
-      <c r="P25" s="92"/>
-      <c r="Q25" s="93"/>
+      <c r="B25" s="82" t="s">
+        <v>52</v>
+      </c>
+      <c r="C25" s="56"/>
+      <c r="D25" s="56"/>
+      <c r="E25" s="56"/>
+      <c r="F25" s="56"/>
+      <c r="G25" s="57"/>
+      <c r="H25" s="54"/>
+      <c r="I25" s="25"/>
+      <c r="J25" s="27"/>
+      <c r="K25" s="64"/>
+      <c r="L25" s="65"/>
+      <c r="M25" s="65"/>
+      <c r="N25" s="65"/>
+      <c r="O25" s="65"/>
+      <c r="P25" s="65"/>
+      <c r="Q25" s="66"/>
       <c r="R25" s="1"/>
     </row>
-    <row r="26" ht="15.75" customHeight="1">
+    <row r="26" spans="1:18" ht="15.75" customHeight="1">
       <c r="A26" s="1"/>
-      <c r="B26" s="90" t="s">
-        <v>51</v>
-      </c>
-      <c r="C26" s="80"/>
-      <c r="D26" s="80"/>
-      <c r="E26" s="80"/>
-      <c r="F26" s="80"/>
-      <c r="G26" s="59"/>
-      <c r="H26" s="10"/>
-      <c r="J26" s="9"/>
-      <c r="K26" s="86"/>
-      <c r="L26" s="3"/>
-      <c r="M26" s="3"/>
-      <c r="N26" s="3"/>
-      <c r="O26" s="3"/>
-      <c r="P26" s="3"/>
-      <c r="Q26" s="4"/>
+      <c r="B26" s="82" t="s">
+        <v>53</v>
+      </c>
+      <c r="C26" s="56"/>
+      <c r="D26" s="56"/>
+      <c r="E26" s="56"/>
+      <c r="F26" s="56"/>
+      <c r="G26" s="57"/>
+      <c r="H26" s="54"/>
+      <c r="I26" s="25"/>
+      <c r="J26" s="27"/>
+      <c r="K26" s="60"/>
+      <c r="L26" s="51"/>
+      <c r="M26" s="51"/>
+      <c r="N26" s="51"/>
+      <c r="O26" s="51"/>
+      <c r="P26" s="51"/>
+      <c r="Q26" s="52"/>
       <c r="R26" s="1"/>
     </row>
-    <row r="27" ht="15.75" customHeight="1">
+    <row r="27" spans="1:18" ht="15.75" customHeight="1">
       <c r="A27" s="1"/>
-      <c r="B27" s="94"/>
-      <c r="C27" s="3"/>
-      <c r="D27" s="3"/>
-      <c r="E27" s="3"/>
-      <c r="F27" s="3"/>
-      <c r="G27" s="4"/>
-      <c r="H27" s="10"/>
-      <c r="J27" s="9"/>
-      <c r="K27" s="10"/>
-      <c r="Q27" s="9"/>
+      <c r="B27" s="79"/>
+      <c r="C27" s="51"/>
+      <c r="D27" s="51"/>
+      <c r="E27" s="51"/>
+      <c r="F27" s="51"/>
+      <c r="G27" s="52"/>
+      <c r="H27" s="54"/>
+      <c r="I27" s="25"/>
+      <c r="J27" s="27"/>
+      <c r="K27" s="54"/>
+      <c r="L27" s="25"/>
+      <c r="M27" s="25"/>
+      <c r="N27" s="25"/>
+      <c r="O27" s="25"/>
+      <c r="P27" s="25"/>
+      <c r="Q27" s="27"/>
       <c r="R27" s="1"/>
     </row>
-    <row r="28" ht="3.75" hidden="1" customHeight="1">
+    <row r="28" spans="1:18" ht="3.75" hidden="1" customHeight="1">
       <c r="A28" s="1"/>
-      <c r="B28" s="10"/>
-      <c r="G28" s="9"/>
-      <c r="H28" s="10"/>
-      <c r="J28" s="9"/>
-      <c r="K28" s="10"/>
-      <c r="Q28" s="9"/>
+      <c r="B28" s="54"/>
+      <c r="C28" s="25"/>
+      <c r="D28" s="25"/>
+      <c r="E28" s="25"/>
+      <c r="F28" s="25"/>
+      <c r="G28" s="27"/>
+      <c r="H28" s="54"/>
+      <c r="I28" s="25"/>
+      <c r="J28" s="27"/>
+      <c r="K28" s="54"/>
+      <c r="L28" s="25"/>
+      <c r="M28" s="25"/>
+      <c r="N28" s="25"/>
+      <c r="O28" s="25"/>
+      <c r="P28" s="25"/>
+      <c r="Q28" s="27"/>
       <c r="R28" s="1"/>
     </row>
-    <row r="29" ht="0.75" customHeight="1">
+    <row r="29" spans="1:18" ht="0.75" customHeight="1">
       <c r="A29" s="1"/>
-      <c r="B29" s="10"/>
-      <c r="G29" s="9"/>
-      <c r="H29" s="10"/>
-      <c r="J29" s="9"/>
-      <c r="K29" s="22"/>
-      <c r="L29" s="18"/>
-      <c r="M29" s="18"/>
-      <c r="N29" s="18"/>
-      <c r="O29" s="18"/>
-      <c r="P29" s="18"/>
-      <c r="Q29" s="23"/>
+      <c r="B29" s="54"/>
+      <c r="C29" s="25"/>
+      <c r="D29" s="25"/>
+      <c r="E29" s="25"/>
+      <c r="F29" s="25"/>
+      <c r="G29" s="27"/>
+      <c r="H29" s="54"/>
+      <c r="I29" s="25"/>
+      <c r="J29" s="27"/>
+      <c r="K29" s="61"/>
+      <c r="L29" s="32"/>
+      <c r="M29" s="32"/>
+      <c r="N29" s="32"/>
+      <c r="O29" s="32"/>
+      <c r="P29" s="32"/>
+      <c r="Q29" s="62"/>
       <c r="R29" s="1"/>
     </row>
-    <row r="30" ht="15.75" customHeight="1">
+    <row r="30" spans="1:18" ht="15.75" customHeight="1">
       <c r="A30" s="1"/>
-      <c r="B30" s="22"/>
-      <c r="C30" s="18"/>
-      <c r="D30" s="18"/>
-      <c r="E30" s="18"/>
-      <c r="F30" s="18"/>
-      <c r="G30" s="23"/>
-      <c r="H30" s="22"/>
-      <c r="I30" s="18"/>
-      <c r="J30" s="23"/>
-      <c r="K30" s="71" t="s">
-        <v>52</v>
-      </c>
-      <c r="L30" s="18"/>
-      <c r="M30" s="18"/>
-      <c r="N30" s="18"/>
-      <c r="O30" s="18"/>
-      <c r="P30" s="18"/>
-      <c r="Q30" s="23"/>
+      <c r="B30" s="61"/>
+      <c r="C30" s="32"/>
+      <c r="D30" s="32"/>
+      <c r="E30" s="32"/>
+      <c r="F30" s="32"/>
+      <c r="G30" s="62"/>
+      <c r="H30" s="61"/>
+      <c r="I30" s="32"/>
+      <c r="J30" s="62"/>
+      <c r="K30" s="31" t="s">
+        <v>44</v>
+      </c>
+      <c r="L30" s="32"/>
+      <c r="M30" s="32"/>
+      <c r="N30" s="32"/>
+      <c r="O30" s="32"/>
+      <c r="P30" s="32"/>
+      <c r="Q30" s="62"/>
       <c r="R30" s="1"/>
     </row>
-    <row r="31" ht="3.75" customHeight="1">
+    <row r="31" spans="1:18" ht="3.75" customHeight="1">
       <c r="A31" s="1"/>
-      <c r="B31" s="95"/>
-      <c r="C31" s="95"/>
-      <c r="D31" s="95"/>
-      <c r="E31" s="95"/>
-      <c r="F31" s="95"/>
-      <c r="G31" s="95"/>
-      <c r="H31" s="95"/>
-      <c r="I31" s="95"/>
-      <c r="J31" s="95"/>
-      <c r="K31" s="95"/>
-      <c r="L31" s="95"/>
-      <c r="M31" s="95"/>
-      <c r="N31" s="95"/>
-      <c r="O31" s="95"/>
-      <c r="P31" s="95"/>
-      <c r="Q31" s="95"/>
+      <c r="B31" s="18"/>
+      <c r="C31" s="18"/>
+      <c r="D31" s="18"/>
+      <c r="E31" s="18"/>
+      <c r="F31" s="18"/>
+      <c r="G31" s="18"/>
+      <c r="H31" s="18"/>
+      <c r="I31" s="18"/>
+      <c r="J31" s="18"/>
+      <c r="K31" s="18"/>
+      <c r="L31" s="18"/>
+      <c r="M31" s="18"/>
+      <c r="N31" s="18"/>
+      <c r="O31" s="18"/>
+      <c r="P31" s="18"/>
+      <c r="Q31" s="18"/>
       <c r="R31" s="1"/>
     </row>
-    <row r="32" ht="15.75" customHeight="1">
-      <c r="B32" s="64" t="s">
-        <v>53</v>
-      </c>
+    <row r="32" spans="1:18" ht="15.75" customHeight="1">
+      <c r="B32" s="46" t="s">
+        <v>45</v>
+      </c>
+      <c r="C32" s="25"/>
+      <c r="D32" s="25"/>
+      <c r="E32" s="25"/>
+      <c r="F32" s="25"/>
+      <c r="G32" s="25"/>
+      <c r="H32" s="25"/>
+      <c r="I32" s="25"/>
+      <c r="J32" s="25"/>
+      <c r="K32" s="25"/>
+      <c r="L32" s="25"/>
+      <c r="M32" s="25"/>
+      <c r="N32" s="25"/>
+      <c r="O32" s="25"/>
+      <c r="P32" s="25"/>
+      <c r="Q32" s="25"/>
     </row>
     <row r="33" ht="15.75" customHeight="1"/>
     <row r="34" ht="15.75" customHeight="1"/>
@@ -2770,19 +3159,23 @@
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="55">
-    <mergeCell ref="K16:L17"/>
-    <mergeCell ref="K19:L19"/>
-    <mergeCell ref="K18:L18"/>
-    <mergeCell ref="B11:Q11"/>
-    <mergeCell ref="B12:Q12"/>
-    <mergeCell ref="I15:O15"/>
-    <mergeCell ref="B13:Q14"/>
-    <mergeCell ref="P16:Q17"/>
-    <mergeCell ref="M16:O16"/>
-    <mergeCell ref="N17:O17"/>
-    <mergeCell ref="N18:O18"/>
-    <mergeCell ref="P15:Q15"/>
-    <mergeCell ref="P18:Q18"/>
+    <mergeCell ref="K30:Q30"/>
+    <mergeCell ref="B32:Q32"/>
+    <mergeCell ref="B27:G30"/>
+    <mergeCell ref="H23:J30"/>
+    <mergeCell ref="P23:Q23"/>
+    <mergeCell ref="K23:O23"/>
+    <mergeCell ref="B26:G26"/>
+    <mergeCell ref="B25:G25"/>
+    <mergeCell ref="B23:G23"/>
+    <mergeCell ref="B24:G24"/>
+    <mergeCell ref="K26:Q29"/>
+    <mergeCell ref="K24:Q25"/>
+    <mergeCell ref="G4:M4"/>
+    <mergeCell ref="B8:I8"/>
+    <mergeCell ref="J8:Q8"/>
+    <mergeCell ref="B6:Q7"/>
+    <mergeCell ref="B21:J22"/>
     <mergeCell ref="B10:H10"/>
     <mergeCell ref="B16:G17"/>
     <mergeCell ref="B15:H15"/>
@@ -2790,21 +3183,23 @@
     <mergeCell ref="B19:G19"/>
     <mergeCell ref="J10:Q10"/>
     <mergeCell ref="B18:G18"/>
-    <mergeCell ref="K26:Q29"/>
-    <mergeCell ref="K24:Q25"/>
-    <mergeCell ref="K30:Q30"/>
-    <mergeCell ref="B32:Q32"/>
-    <mergeCell ref="B27:G30"/>
-    <mergeCell ref="H23:J30"/>
-    <mergeCell ref="P23:Q23"/>
-    <mergeCell ref="K23:O23"/>
-    <mergeCell ref="B21:J22"/>
-    <mergeCell ref="B23:G23"/>
-    <mergeCell ref="B24:G24"/>
+    <mergeCell ref="N18:O18"/>
+    <mergeCell ref="P15:Q15"/>
+    <mergeCell ref="B11:Q11"/>
+    <mergeCell ref="B2:Q2"/>
+    <mergeCell ref="B3:C4"/>
     <mergeCell ref="K22:O22"/>
     <mergeCell ref="P22:Q22"/>
-    <mergeCell ref="B26:G26"/>
-    <mergeCell ref="B25:G25"/>
+    <mergeCell ref="P18:Q18"/>
+    <mergeCell ref="B12:Q12"/>
+    <mergeCell ref="I15:O15"/>
+    <mergeCell ref="B13:Q14"/>
+    <mergeCell ref="P16:Q17"/>
+    <mergeCell ref="M16:O16"/>
+    <mergeCell ref="N17:O17"/>
+    <mergeCell ref="K16:L17"/>
+    <mergeCell ref="P21:Q21"/>
+    <mergeCell ref="K21:O21"/>
     <mergeCell ref="F3:N3"/>
     <mergeCell ref="O3:Q4"/>
     <mergeCell ref="H16:H17"/>
@@ -2817,18 +3212,11 @@
     <mergeCell ref="B9:I9"/>
     <mergeCell ref="J9:Q9"/>
     <mergeCell ref="G5:M5"/>
-    <mergeCell ref="G4:M4"/>
-    <mergeCell ref="B8:I8"/>
-    <mergeCell ref="J8:Q8"/>
-    <mergeCell ref="B6:Q7"/>
-    <mergeCell ref="B2:Q2"/>
-    <mergeCell ref="B3:C4"/>
-    <mergeCell ref="P21:Q21"/>
-    <mergeCell ref="K21:O21"/>
+    <mergeCell ref="K19:L19"/>
+    <mergeCell ref="K18:L18"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.25" right="0.25" top="0.75"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add TDS amount in the addvance receipt #CRMS-2286
</commit_message>
<xml_diff>
--- a/application/controllers/excel-templates/247around_Tax_Invoice_Inter_State.xlsx
+++ b/application/controllers/excel-templates/247around_Tax_Invoice_Inter_State.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="58">
   <si>
     <t>{meta:main_company_name}</t>
   </si>
@@ -134,7 +134,7 @@
     <t>Total Amt before Tax</t>
   </si>
   <si>
-    <t xml:space="preserve">{meta:total_taxable_value}	</t>
+    <t xml:space="preserve">{meta:total_taxable_value}        </t>
   </si>
   <si>
     <t>{meta:price_inword}</t>
@@ -150,6 +150,12 @@
   </si>
   <si>
     <t>{meta:tcs_amount}</t>
+  </si>
+  <si>
+    <t>{meta:tds_text}</t>
+  </si>
+  <si>
+    <t>{meta:tds_amount}</t>
   </si>
   <si>
     <t>Total Amount</t>
@@ -259,7 +265,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="53">
+  <borders count="49">
     <border/>
     <border>
       <left style="medium">
@@ -687,35 +693,13 @@
       <top style="medium">
         <color rgb="FF000000"/>
       </top>
-      <bottom/>
-    </border>
-    <border>
-      <right/>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <bottom/>
-    </border>
-    <border>
-      <bottom/>
-    </border>
-    <border>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
       <bottom/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="96">
+  <cellXfs count="92">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -872,9 +856,6 @@
     <xf borderId="13" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="13" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
     <xf borderId="6" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -883,7 +864,7 @@
     </xf>
     <xf borderId="42" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="22" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
@@ -896,36 +877,35 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf borderId="44" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf borderId="45" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="44" fillId="0" fontId="9" numFmtId="1" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf borderId="46" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="7" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="44" fillId="0" fontId="9" numFmtId="1" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
-    <xf borderId="46" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="13" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf borderId="47" fillId="2" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf borderId="48" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="49" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="1" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="6" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
     <xf borderId="1" fillId="2" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="44" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf borderId="50" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="51" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="52" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="1" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1599,7 +1579,7 @@
         <v>36</v>
       </c>
       <c r="O19" s="66"/>
-      <c r="P19" s="70" t="s">
+      <c r="P19" s="69" t="s">
         <v>37</v>
       </c>
       <c r="Q19" s="29"/>
@@ -1607,7 +1587,7 @@
     </row>
     <row r="20" ht="21.75" customHeight="1">
       <c r="A20" s="1"/>
-      <c r="B20" s="71" t="s">
+      <c r="B20" s="70" t="s">
         <v>38</v>
       </c>
       <c r="C20" s="18"/>
@@ -1618,14 +1598,14 @@
       <c r="H20" s="18"/>
       <c r="I20" s="18"/>
       <c r="J20" s="18"/>
-      <c r="K20" s="72" t="s">
+      <c r="K20" s="71" t="s">
         <v>39</v>
       </c>
       <c r="L20" s="40"/>
       <c r="M20" s="40"/>
       <c r="N20" s="40"/>
-      <c r="O20" s="73"/>
-      <c r="P20" s="74" t="s">
+      <c r="O20" s="72"/>
+      <c r="P20" s="73" t="s">
         <v>40</v>
       </c>
       <c r="Q20" s="41"/>
@@ -1633,7 +1613,7 @@
     </row>
     <row r="21" ht="15.75" customHeight="1">
       <c r="A21" s="1"/>
-      <c r="B21" s="75" t="s">
+      <c r="B21" s="74" t="s">
         <v>41</v>
       </c>
       <c r="C21" s="3"/>
@@ -1644,14 +1624,14 @@
       <c r="H21" s="3"/>
       <c r="I21" s="3"/>
       <c r="J21" s="4"/>
-      <c r="K21" s="76" t="s">
+      <c r="K21" s="75" t="s">
         <v>42</v>
       </c>
       <c r="L21" s="31"/>
       <c r="M21" s="31"/>
       <c r="N21" s="31"/>
-      <c r="O21" s="77"/>
-      <c r="P21" s="78" t="s">
+      <c r="O21" s="76"/>
+      <c r="P21" s="77" t="s">
         <v>43</v>
       </c>
       <c r="Q21" s="32"/>
@@ -1661,187 +1641,177 @@
       <c r="A22" s="1"/>
       <c r="B22" s="10"/>
       <c r="J22" s="9"/>
-      <c r="K22" s="79" t="s">
+      <c r="K22" s="78" t="s">
         <v>44</v>
       </c>
-      <c r="L22" s="80"/>
-      <c r="M22" s="80"/>
-      <c r="N22" s="80"/>
+      <c r="L22" s="79"/>
+      <c r="M22" s="79"/>
+      <c r="N22" s="79"/>
       <c r="O22" s="59"/>
-      <c r="P22" s="81" t="s">
+      <c r="P22" s="80" t="s">
         <v>45</v>
       </c>
-      <c r="Q22" s="82"/>
+      <c r="Q22" s="81"/>
       <c r="R22" s="1"/>
     </row>
     <row r="23" ht="21.0" customHeight="1">
       <c r="A23" s="1"/>
-      <c r="B23" s="22"/>
-      <c r="C23" s="18"/>
-      <c r="D23" s="18"/>
-      <c r="E23" s="18"/>
-      <c r="F23" s="18"/>
-      <c r="G23" s="18"/>
-      <c r="H23" s="18"/>
-      <c r="I23" s="18"/>
-      <c r="J23" s="23"/>
-      <c r="K23" s="83" t="s">
+      <c r="B23" s="10"/>
+      <c r="J23" s="9"/>
+      <c r="K23" s="82" t="s">
         <v>46</v>
       </c>
-      <c r="L23" s="28"/>
-      <c r="M23" s="28"/>
-      <c r="N23" s="28"/>
-      <c r="O23" s="29"/>
-      <c r="P23" s="81" t="s">
+      <c r="L23" s="18"/>
+      <c r="M23" s="18"/>
+      <c r="N23" s="18"/>
+      <c r="O23" s="18"/>
+      <c r="P23" s="83" t="s">
         <v>47</v>
       </c>
-      <c r="Q23" s="82"/>
+      <c r="Q23" s="81"/>
       <c r="R23" s="1"/>
     </row>
-    <row r="24" ht="24.0" customHeight="1">
+    <row r="24" ht="21.0" customHeight="1">
       <c r="A24" s="1"/>
-      <c r="B24" s="84" t="s">
+      <c r="B24" s="22"/>
+      <c r="C24" s="18"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="18"/>
+      <c r="F24" s="18"/>
+      <c r="G24" s="18"/>
+      <c r="H24" s="18"/>
+      <c r="I24" s="18"/>
+      <c r="J24" s="23"/>
+      <c r="K24" s="84" t="s">
         <v>48</v>
       </c>
-      <c r="C24" s="85"/>
-      <c r="D24" s="85"/>
-      <c r="E24" s="85"/>
-      <c r="F24" s="85"/>
-      <c r="G24" s="86"/>
-      <c r="H24" s="87"/>
-      <c r="I24" s="3"/>
-      <c r="J24" s="4"/>
-      <c r="K24" s="79" t="s">
+      <c r="L24" s="28"/>
+      <c r="M24" s="28"/>
+      <c r="N24" s="28"/>
+      <c r="O24" s="29"/>
+      <c r="P24" s="80" t="s">
         <v>49</v>
       </c>
-      <c r="L24" s="80"/>
-      <c r="M24" s="80"/>
-      <c r="N24" s="80"/>
-      <c r="O24" s="59"/>
-      <c r="P24" s="88">
+      <c r="Q24" s="81"/>
+      <c r="R24" s="1"/>
+    </row>
+    <row r="25" ht="24.0" customHeight="1">
+      <c r="A25" s="1"/>
+      <c r="B25" s="85" t="s">
+        <v>50</v>
+      </c>
+      <c r="C25" s="86"/>
+      <c r="D25" s="86"/>
+      <c r="E25" s="86"/>
+      <c r="F25" s="86"/>
+      <c r="G25" s="86"/>
+      <c r="H25" s="87"/>
+      <c r="I25" s="3"/>
+      <c r="J25" s="4"/>
+      <c r="K25" s="78" t="s">
+        <v>51</v>
+      </c>
+      <c r="L25" s="79"/>
+      <c r="M25" s="79"/>
+      <c r="N25" s="79"/>
+      <c r="O25" s="59"/>
+      <c r="P25" s="70">
         <v>0.0</v>
       </c>
-      <c r="Q24" s="23"/>
-      <c r="R24" s="1"/>
-    </row>
-    <row r="25" ht="15.75" customHeight="1">
-      <c r="A25" s="1"/>
-      <c r="B25" s="24" t="s">
-        <v>50</v>
-      </c>
-      <c r="C25" s="25"/>
-      <c r="D25" s="25"/>
-      <c r="E25" s="25"/>
-      <c r="F25" s="25"/>
-      <c r="G25" s="52"/>
-      <c r="H25" s="10"/>
-      <c r="J25" s="9"/>
-      <c r="K25" s="89" t="s">
-        <v>51</v>
-      </c>
-      <c r="L25" s="3"/>
-      <c r="M25" s="3"/>
-      <c r="N25" s="3"/>
-      <c r="O25" s="3"/>
-      <c r="P25" s="3"/>
-      <c r="Q25" s="4"/>
+      <c r="Q25" s="23"/>
       <c r="R25" s="1"/>
     </row>
     <row r="26" ht="15.75" customHeight="1">
       <c r="A26" s="1"/>
-      <c r="B26" s="90" t="s">
+      <c r="B26" s="24" t="s">
         <v>52</v>
       </c>
-      <c r="C26" s="80"/>
-      <c r="D26" s="80"/>
-      <c r="E26" s="80"/>
-      <c r="F26" s="80"/>
-      <c r="G26" s="59"/>
+      <c r="C26" s="25"/>
+      <c r="D26" s="25"/>
+      <c r="E26" s="25"/>
+      <c r="F26" s="25"/>
+      <c r="G26" s="52"/>
       <c r="H26" s="10"/>
       <c r="J26" s="9"/>
-      <c r="K26" s="91"/>
-      <c r="L26" s="92"/>
-      <c r="M26" s="92"/>
-      <c r="N26" s="92"/>
-      <c r="O26" s="92"/>
-      <c r="P26" s="92"/>
-      <c r="Q26" s="93"/>
+      <c r="K26" s="88" t="s">
+        <v>53</v>
+      </c>
+      <c r="L26" s="3"/>
+      <c r="M26" s="3"/>
+      <c r="N26" s="3"/>
+      <c r="O26" s="3"/>
+      <c r="P26" s="3"/>
+      <c r="Q26" s="4"/>
       <c r="R26" s="1"/>
     </row>
     <row r="27" ht="15.75" customHeight="1">
       <c r="A27" s="1"/>
-      <c r="B27" s="90" t="s">
-        <v>53</v>
-      </c>
-      <c r="C27" s="80"/>
-      <c r="D27" s="80"/>
-      <c r="E27" s="80"/>
-      <c r="F27" s="80"/>
+      <c r="B27" s="89" t="s">
+        <v>54</v>
+      </c>
+      <c r="C27" s="79"/>
+      <c r="D27" s="79"/>
+      <c r="E27" s="79"/>
+      <c r="F27" s="79"/>
       <c r="G27" s="59"/>
       <c r="H27" s="10"/>
       <c r="J27" s="9"/>
-      <c r="K27" s="87"/>
-      <c r="L27" s="3"/>
-      <c r="M27" s="3"/>
-      <c r="N27" s="3"/>
-      <c r="O27" s="3"/>
-      <c r="P27" s="3"/>
-      <c r="Q27" s="4"/>
+      <c r="K27" s="10"/>
+      <c r="Q27" s="9"/>
       <c r="R27" s="1"/>
     </row>
     <row r="28" ht="15.75" customHeight="1">
       <c r="A28" s="1"/>
-      <c r="B28" s="94"/>
-      <c r="C28" s="3"/>
-      <c r="D28" s="3"/>
-      <c r="E28" s="3"/>
-      <c r="F28" s="3"/>
-      <c r="G28" s="4"/>
+      <c r="B28" s="89" t="s">
+        <v>55</v>
+      </c>
+      <c r="C28" s="79"/>
+      <c r="D28" s="79"/>
+      <c r="E28" s="79"/>
+      <c r="F28" s="79"/>
+      <c r="G28" s="59"/>
       <c r="H28" s="10"/>
       <c r="J28" s="9"/>
-      <c r="K28" s="10"/>
-      <c r="Q28" s="9"/>
+      <c r="K28" s="87"/>
+      <c r="L28" s="3"/>
+      <c r="M28" s="3"/>
+      <c r="N28" s="3"/>
+      <c r="O28" s="3"/>
+      <c r="P28" s="3"/>
+      <c r="Q28" s="4"/>
       <c r="R28" s="1"/>
     </row>
-    <row r="29" ht="3.75" hidden="1" customHeight="1">
+    <row r="29" ht="15.75" customHeight="1">
       <c r="A29" s="1"/>
-      <c r="B29" s="10"/>
-      <c r="G29" s="9"/>
+      <c r="B29" s="90"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="3"/>
+      <c r="G29" s="4"/>
       <c r="H29" s="10"/>
       <c r="J29" s="9"/>
       <c r="K29" s="10"/>
       <c r="Q29" s="9"/>
       <c r="R29" s="1"/>
     </row>
-    <row r="30" ht="0.75" customHeight="1">
+    <row r="30" ht="3.75" hidden="1" customHeight="1">
       <c r="A30" s="1"/>
       <c r="B30" s="10"/>
       <c r="G30" s="9"/>
       <c r="H30" s="10"/>
       <c r="J30" s="9"/>
-      <c r="K30" s="22"/>
-      <c r="L30" s="18"/>
-      <c r="M30" s="18"/>
-      <c r="N30" s="18"/>
-      <c r="O30" s="18"/>
-      <c r="P30" s="18"/>
-      <c r="Q30" s="23"/>
+      <c r="K30" s="10"/>
+      <c r="Q30" s="9"/>
       <c r="R30" s="1"/>
     </row>
-    <row r="31" ht="15.75" customHeight="1">
+    <row r="31" ht="0.75" customHeight="1">
       <c r="A31" s="1"/>
-      <c r="B31" s="22"/>
-      <c r="C31" s="18"/>
-      <c r="D31" s="18"/>
-      <c r="E31" s="18"/>
-      <c r="F31" s="18"/>
-      <c r="G31" s="23"/>
-      <c r="H31" s="22"/>
-      <c r="I31" s="18"/>
-      <c r="J31" s="23"/>
-      <c r="K31" s="71" t="s">
-        <v>54</v>
-      </c>
+      <c r="B31" s="10"/>
+      <c r="G31" s="9"/>
+      <c r="H31" s="10"/>
+      <c r="J31" s="9"/>
+      <c r="K31" s="22"/>
       <c r="L31" s="18"/>
       <c r="M31" s="18"/>
       <c r="N31" s="18"/>
@@ -1850,32 +1820,53 @@
       <c r="Q31" s="23"/>
       <c r="R31" s="1"/>
     </row>
-    <row r="32" ht="3.75" customHeight="1">
+    <row r="32" ht="15.75" customHeight="1">
       <c r="A32" s="1"/>
-      <c r="B32" s="95"/>
-      <c r="C32" s="95"/>
-      <c r="D32" s="95"/>
-      <c r="E32" s="95"/>
-      <c r="F32" s="95"/>
-      <c r="G32" s="95"/>
-      <c r="H32" s="95"/>
-      <c r="I32" s="95"/>
-      <c r="J32" s="95"/>
-      <c r="K32" s="95"/>
-      <c r="L32" s="95"/>
-      <c r="M32" s="95"/>
-      <c r="N32" s="95"/>
-      <c r="O32" s="95"/>
-      <c r="P32" s="95"/>
-      <c r="Q32" s="95"/>
+      <c r="B32" s="22"/>
+      <c r="C32" s="18"/>
+      <c r="D32" s="18"/>
+      <c r="E32" s="18"/>
+      <c r="F32" s="18"/>
+      <c r="G32" s="23"/>
+      <c r="H32" s="22"/>
+      <c r="I32" s="18"/>
+      <c r="J32" s="23"/>
+      <c r="K32" s="70" t="s">
+        <v>56</v>
+      </c>
+      <c r="L32" s="18"/>
+      <c r="M32" s="18"/>
+      <c r="N32" s="18"/>
+      <c r="O32" s="18"/>
+      <c r="P32" s="18"/>
+      <c r="Q32" s="23"/>
       <c r="R32" s="1"/>
     </row>
-    <row r="33" ht="15.75" customHeight="1">
-      <c r="B33" s="64" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="34" ht="15.75" customHeight="1"/>
+    <row r="33" ht="3.75" customHeight="1">
+      <c r="A33" s="1"/>
+      <c r="B33" s="91"/>
+      <c r="C33" s="91"/>
+      <c r="D33" s="91"/>
+      <c r="E33" s="91"/>
+      <c r="F33" s="91"/>
+      <c r="G33" s="91"/>
+      <c r="H33" s="91"/>
+      <c r="I33" s="91"/>
+      <c r="J33" s="91"/>
+      <c r="K33" s="91"/>
+      <c r="L33" s="91"/>
+      <c r="M33" s="91"/>
+      <c r="N33" s="91"/>
+      <c r="O33" s="91"/>
+      <c r="P33" s="91"/>
+      <c r="Q33" s="91"/>
+      <c r="R33" s="1"/>
+    </row>
+    <row r="34" ht="15.75" customHeight="1">
+      <c r="B34" s="64" t="s">
+        <v>57</v>
+      </c>
+    </row>
     <row r="35" ht="15.75" customHeight="1"/>
     <row r="36" ht="15.75" customHeight="1"/>
     <row r="37" ht="15.75" customHeight="1"/>
@@ -2844,18 +2835,28 @@
     <row r="1000" ht="15.75" customHeight="1"/>
     <row r="1001" ht="15.75" customHeight="1"/>
   </sheetData>
-  <mergeCells count="57">
+  <mergeCells count="59">
+    <mergeCell ref="K24:O24"/>
+    <mergeCell ref="K25:O25"/>
+    <mergeCell ref="P25:Q25"/>
     <mergeCell ref="K23:O23"/>
     <mergeCell ref="P23:Q23"/>
-    <mergeCell ref="P24:Q24"/>
     <mergeCell ref="K20:O20"/>
     <mergeCell ref="P20:Q20"/>
     <mergeCell ref="K21:O21"/>
     <mergeCell ref="P21:Q21"/>
     <mergeCell ref="K22:O22"/>
     <mergeCell ref="P22:Q22"/>
-    <mergeCell ref="K24:O24"/>
-    <mergeCell ref="K25:Q26"/>
+    <mergeCell ref="P24:Q24"/>
+    <mergeCell ref="N19:O19"/>
+    <mergeCell ref="P19:Q19"/>
+    <mergeCell ref="K16:L17"/>
+    <mergeCell ref="M16:O16"/>
+    <mergeCell ref="N17:O17"/>
+    <mergeCell ref="K18:L18"/>
+    <mergeCell ref="N18:O18"/>
+    <mergeCell ref="P18:Q18"/>
+    <mergeCell ref="K19:L19"/>
     <mergeCell ref="B2:Q2"/>
     <mergeCell ref="B3:C4"/>
     <mergeCell ref="F3:N3"/>
@@ -2872,7 +2873,7 @@
     <mergeCell ref="B11:Q11"/>
     <mergeCell ref="I16:I17"/>
     <mergeCell ref="J16:J17"/>
-    <mergeCell ref="H24:J31"/>
+    <mergeCell ref="H25:J32"/>
     <mergeCell ref="B12:Q12"/>
     <mergeCell ref="B13:Q14"/>
     <mergeCell ref="B15:H15"/>
@@ -2880,28 +2881,20 @@
     <mergeCell ref="P15:Q15"/>
     <mergeCell ref="H16:H17"/>
     <mergeCell ref="P16:Q17"/>
-    <mergeCell ref="N19:O19"/>
-    <mergeCell ref="P19:Q19"/>
-    <mergeCell ref="K16:L17"/>
-    <mergeCell ref="M16:O16"/>
-    <mergeCell ref="N17:O17"/>
-    <mergeCell ref="K18:L18"/>
-    <mergeCell ref="N18:O18"/>
-    <mergeCell ref="P18:Q18"/>
-    <mergeCell ref="K19:L19"/>
-    <mergeCell ref="B26:G26"/>
     <mergeCell ref="B27:G27"/>
-    <mergeCell ref="K27:Q30"/>
-    <mergeCell ref="B28:G31"/>
-    <mergeCell ref="K31:Q31"/>
-    <mergeCell ref="B33:Q33"/>
+    <mergeCell ref="B28:G28"/>
+    <mergeCell ref="B29:G32"/>
+    <mergeCell ref="B34:Q34"/>
     <mergeCell ref="B16:G17"/>
     <mergeCell ref="B18:G18"/>
     <mergeCell ref="B19:G19"/>
     <mergeCell ref="B20:J20"/>
-    <mergeCell ref="B24:G24"/>
     <mergeCell ref="B25:G25"/>
-    <mergeCell ref="B21:J23"/>
+    <mergeCell ref="B26:G26"/>
+    <mergeCell ref="B21:J24"/>
+    <mergeCell ref="K26:Q27"/>
+    <mergeCell ref="K28:Q31"/>
+    <mergeCell ref="K32:Q32"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.25" right="0.25" top="0.75"/>

</xml_diff>